<commit_message>
Grafikler klasörü eklendi ve analiz dosyaları güncellendi
</commit_message>
<xml_diff>
--- a/TSLA_1y_analysis.xlsx
+++ b/TSLA_1y_analysis.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J253"/>
+  <dimension ref="A1:G253"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,21 +475,6 @@
           <t>Daily Return</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>SMA_20</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>SMA_50</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>RSI</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -523,9 +508,6 @@
         </is>
       </c>
       <c r="G2" s="1" t="inlineStr"/>
-      <c r="H2" s="1" t="inlineStr"/>
-      <c r="I2" s="1" t="inlineStr"/>
-      <c r="J2" s="1" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -554,9 +536,6 @@
         <v>146912900</v>
       </c>
       <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
@@ -580,9 +559,6 @@
       <c r="G5" t="n">
         <v>0.01551614225148668</v>
       </c>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
@@ -606,9 +582,6 @@
       <c r="G6" t="n">
         <v>-0.03141564404151898</v>
       </c>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
@@ -632,9 +605,6 @@
       <c r="G7" t="n">
         <v>0.002937608561525362</v>
       </c>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
@@ -658,9 +628,6 @@
       <c r="G8" t="n">
         <v>-0.04024394716220991</v>
       </c>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
@@ -684,9 +651,6 @@
       <c r="G9" t="n">
         <v>0.05146320115237035</v>
       </c>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
@@ -710,9 +674,6 @@
       <c r="G10" t="n">
         <v>-0.0203967624987722</v>
       </c>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
@@ -736,9 +697,6 @@
       <c r="G11" t="n">
         <v>-0.123346045894037</v>
       </c>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
@@ -762,9 +720,6 @@
       <c r="G12" t="n">
         <v>0.01972310939623889</v>
       </c>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
@@ -788,9 +743,6 @@
       <c r="G13" t="n">
         <v>-0.00204311894775111</v>
       </c>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
@@ -814,9 +766,6 @@
       <c r="G14" t="n">
         <v>0.05595997671056185</v>
       </c>
-      <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
@@ -840,9 +789,6 @@
       <c r="G15" t="n">
         <v>-0.04084450985365373</v>
       </c>
-      <c r="H15" t="inlineStr"/>
-      <c r="I15" t="inlineStr"/>
-      <c r="J15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
@@ -866,9 +812,6 @@
       <c r="G16" t="n">
         <v>0.04244907202543402</v>
       </c>
-      <c r="H16" t="inlineStr"/>
-      <c r="I16" t="inlineStr"/>
-      <c r="J16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
@@ -892,9 +835,6 @@
       <c r="G17" t="n">
         <v>-0.06554059651757449</v>
       </c>
-      <c r="H17" t="inlineStr"/>
-      <c r="I17" t="inlineStr"/>
-      <c r="J17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
@@ -918,11 +858,6 @@
       <c r="G18" t="n">
         <v>-0.04237758192170538</v>
       </c>
-      <c r="H18" t="inlineStr"/>
-      <c r="I18" t="inlineStr"/>
-      <c r="J18" t="n">
-        <v>32.8240776248182</v>
-      </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
@@ -946,11 +881,6 @@
       <c r="G19" t="n">
         <v>-0.04232673647438423</v>
       </c>
-      <c r="H19" t="inlineStr"/>
-      <c r="I19" t="inlineStr"/>
-      <c r="J19" t="n">
-        <v>28.75976093889315</v>
-      </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
@@ -974,11 +904,6 @@
       <c r="G20" t="n">
         <v>0.008849529684359148</v>
       </c>
-      <c r="H20" t="inlineStr"/>
-      <c r="I20" t="inlineStr"/>
-      <c r="J20" t="n">
-        <v>31.51838037164369</v>
-      </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
@@ -1002,11 +927,6 @@
       <c r="G21" t="n">
         <v>-0.04425839767656337</v>
       </c>
-      <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr"/>
-      <c r="J21" t="n">
-        <v>29.12155809714714</v>
-      </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
@@ -1030,11 +950,6 @@
       <c r="G22" t="n">
         <v>0.03692116204562312</v>
       </c>
-      <c r="H22" t="inlineStr"/>
-      <c r="I22" t="inlineStr"/>
-      <c r="J22" t="n">
-        <v>35.01633567249303</v>
-      </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
@@ -1058,13 +973,6 @@
       <c r="G23" t="n">
         <v>0.005833854775063374</v>
       </c>
-      <c r="H23" t="n">
-        <v>225.075</v>
-      </c>
-      <c r="I23" t="inlineStr"/>
-      <c r="J23" t="n">
-        <v>29.15081816029151</v>
-      </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
@@ -1088,13 +996,6 @@
       <c r="G24" t="n">
         <v>-0.01254997253417967</v>
       </c>
-      <c r="H24" t="n">
-        <v>222.3175003051758</v>
-      </c>
-      <c r="I24" t="inlineStr"/>
-      <c r="J24" t="n">
-        <v>29.78248625466134</v>
-      </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
@@ -1118,13 +1019,6 @@
       <c r="G25" t="n">
         <v>0.05235706137163754</v>
       </c>
-      <c r="H25" t="n">
-        <v>219.8810005187988</v>
-      </c>
-      <c r="I25" t="inlineStr"/>
-      <c r="J25" t="n">
-        <v>45.95478763720578</v>
-      </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
@@ -1148,13 +1042,6 @@
       <c r="G26" t="n">
         <v>-0.0310349655555765</v>
       </c>
-      <c r="H26" t="n">
-        <v>217.5250007629394</v>
-      </c>
-      <c r="I26" t="inlineStr"/>
-      <c r="J26" t="n">
-        <v>40.84425435989651</v>
-      </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
@@ -1178,13 +1065,6 @@
       <c r="G27" t="n">
         <v>0.06336276788880446</v>
       </c>
-      <c r="H27" t="n">
-        <v>215.7705009460449</v>
-      </c>
-      <c r="I27" t="inlineStr"/>
-      <c r="J27" t="n">
-        <v>47.54680873634334</v>
-      </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
@@ -1208,13 +1088,6 @@
       <c r="G28" t="n">
         <v>0.009246267550119258</v>
       </c>
-      <c r="H28" t="n">
-        <v>214.6165008544922</v>
-      </c>
-      <c r="I28" t="inlineStr"/>
-      <c r="J28" t="n">
-        <v>42.39336934198075</v>
-      </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
@@ -1238,13 +1111,6 @@
       <c r="G29" t="n">
         <v>0.03053861860369222</v>
       </c>
-      <c r="H29" t="n">
-        <v>213.1770011901855</v>
-      </c>
-      <c r="I29" t="inlineStr"/>
-      <c r="J29" t="n">
-        <v>50.04894582024799</v>
-      </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
@@ -1268,13 +1134,6 @@
       <c r="G30" t="n">
         <v>-0.007273684933137958</v>
       </c>
-      <c r="H30" t="n">
-        <v>211.9130012512207</v>
-      </c>
-      <c r="I30" t="inlineStr"/>
-      <c r="J30" t="n">
-        <v>44.1853054265522</v>
-      </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
@@ -1298,13 +1157,6 @@
       <c r="G31" t="n">
         <v>0.009814554993405888</v>
       </c>
-      <c r="H31" t="n">
-        <v>212.2770011901856</v>
-      </c>
-      <c r="I31" t="inlineStr"/>
-      <c r="J31" t="n">
-        <v>53.9426776938931</v>
-      </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
@@ -1328,13 +1180,6 @@
       <c r="G32" t="n">
         <v>-0.05647870456867699</v>
       </c>
-      <c r="H32" t="n">
-        <v>211.797501373291</v>
-      </c>
-      <c r="I32" t="inlineStr"/>
-      <c r="J32" t="n">
-        <v>51.76484850275229</v>
-      </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
@@ -1358,13 +1203,6 @@
       <c r="G33" t="n">
         <v>0.04585589810206048</v>
       </c>
-      <c r="H33" t="n">
-        <v>211.8235015869141</v>
-      </c>
-      <c r="I33" t="inlineStr"/>
-      <c r="J33" t="n">
-        <v>62.52629458132822</v>
-      </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
@@ -1388,13 +1226,6 @@
       <c r="G34" t="n">
         <v>-0.0322712435275504</v>
       </c>
-      <c r="H34" t="n">
-        <v>210.8790016174316</v>
-      </c>
-      <c r="I34" t="inlineStr"/>
-      <c r="J34" t="n">
-        <v>56.91191484477415</v>
-      </c>
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
@@ -1418,13 +1249,6 @@
       <c r="G35" t="n">
         <v>-0.01876084552339086</v>
       </c>
-      <c r="H35" t="n">
-        <v>210.2085021972656</v>
-      </c>
-      <c r="I35" t="inlineStr"/>
-      <c r="J35" t="n">
-        <v>60.13946233729571</v>
-      </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="n">
@@ -1448,13 +1272,6 @@
       <c r="G36" t="n">
         <v>-0.01653843794670573</v>
       </c>
-      <c r="H36" t="n">
-        <v>208.8925018310547</v>
-      </c>
-      <c r="I36" t="inlineStr"/>
-      <c r="J36" t="n">
-        <v>54.19143775087318</v>
-      </c>
     </row>
     <row r="37">
       <c r="A37" s="2" t="n">
@@ -1478,13 +1295,6 @@
       <c r="G37" t="n">
         <v>0.002575935743848623</v>
       </c>
-      <c r="H37" t="n">
-        <v>208.3635017395019</v>
-      </c>
-      <c r="I37" t="inlineStr"/>
-      <c r="J37" t="n">
-        <v>53.83863063353457</v>
-      </c>
     </row>
     <row r="38">
       <c r="A38" s="2" t="n">
@@ -1508,13 +1318,6 @@
       <c r="G38" t="n">
         <v>0.03795812428442069</v>
       </c>
-      <c r="H38" t="n">
-        <v>208.6855018615723</v>
-      </c>
-      <c r="I38" t="inlineStr"/>
-      <c r="J38" t="n">
-        <v>59.5385652253719</v>
-      </c>
     </row>
     <row r="39">
       <c r="A39" s="2" t="n">
@@ -1538,13 +1341,6 @@
       <c r="G39" t="n">
         <v>-0.01639341692041563</v>
       </c>
-      <c r="H39" t="n">
-        <v>209.2715019226074</v>
-      </c>
-      <c r="I39" t="inlineStr"/>
-      <c r="J39" t="n">
-        <v>51.72499969117531</v>
-      </c>
     </row>
     <row r="40">
       <c r="A40" s="2" t="n">
@@ -1568,13 +1364,6 @@
       <c r="G40" t="n">
         <v>0.04183284569452206</v>
       </c>
-      <c r="H40" t="n">
-        <v>210.2100021362305</v>
-      </c>
-      <c r="I40" t="inlineStr"/>
-      <c r="J40" t="n">
-        <v>60.90744108334641</v>
-      </c>
     </row>
     <row r="41">
       <c r="A41" s="2" t="n">
@@ -1598,13 +1387,6 @@
       <c r="G41" t="n">
         <v>0.04904058305110959</v>
       </c>
-      <c r="H41" t="n">
-        <v>212.1305023193359</v>
-      </c>
-      <c r="I41" t="inlineStr"/>
-      <c r="J41" t="n">
-        <v>59.938003715085</v>
-      </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="n">
@@ -1628,13 +1410,6 @@
       <c r="G42" t="n">
         <v>-0.0844593239607937</v>
       </c>
-      <c r="H42" t="n">
-        <v>212.7250022888184</v>
-      </c>
-      <c r="I42" t="inlineStr"/>
-      <c r="J42" t="n">
-        <v>47.2530836020198</v>
-      </c>
     </row>
     <row r="43">
       <c r="A43" s="2" t="n">
@@ -1658,13 +1433,6 @@
       <c r="G43" t="n">
         <v>0.02628960592816965</v>
       </c>
-      <c r="H43" t="n">
-        <v>213.5385025024414</v>
-      </c>
-      <c r="I43" t="inlineStr"/>
-      <c r="J43" t="n">
-        <v>46.67697231044787</v>
-      </c>
     </row>
     <row r="44">
       <c r="A44" s="2" t="n">
@@ -1688,13 +1456,6 @@
       <c r="G44" t="n">
         <v>0.04577608406578748</v>
       </c>
-      <c r="H44" t="n">
-        <v>214.9725021362305</v>
-      </c>
-      <c r="I44" t="inlineStr"/>
-      <c r="J44" t="n">
-        <v>52.40671792333288</v>
-      </c>
     </row>
     <row r="45">
       <c r="A45" s="2" t="n">
@@ -1718,13 +1479,6 @@
       <c r="G45" t="n">
         <v>0.008666077418469476</v>
       </c>
-      <c r="H45" t="n">
-        <v>215.9875022888183</v>
-      </c>
-      <c r="I45" t="inlineStr"/>
-      <c r="J45" t="n">
-        <v>52.3116438977551</v>
-      </c>
     </row>
     <row r="46">
       <c r="A46" s="2" t="n">
@@ -1748,13 +1502,6 @@
       <c r="G46" t="n">
         <v>0.007364189890953776</v>
       </c>
-      <c r="H46" t="n">
-        <v>217.4090019226074</v>
-      </c>
-      <c r="I46" t="inlineStr"/>
-      <c r="J46" t="n">
-        <v>60.16561917407169</v>
-      </c>
     </row>
     <row r="47">
       <c r="A47" s="2" t="n">
@@ -1778,13 +1525,6 @@
       <c r="G47" t="n">
         <v>0.00208866338557212</v>
       </c>
-      <c r="H47" t="n">
-        <v>218.2165016174316</v>
-      </c>
-      <c r="I47" t="inlineStr"/>
-      <c r="J47" t="n">
-        <v>55.86400812031128</v>
-      </c>
     </row>
     <row r="48">
       <c r="A48" s="2" t="n">
@@ -1808,13 +1548,6 @@
       <c r="G48" t="n">
         <v>-0.01524162842140864</v>
       </c>
-      <c r="H48" t="n">
-        <v>218.7495018005371</v>
-      </c>
-      <c r="I48" t="inlineStr"/>
-      <c r="J48" t="n">
-        <v>58.33435327259932</v>
-      </c>
     </row>
     <row r="49">
       <c r="A49" s="2" t="n">
@@ -1838,13 +1571,6 @@
       <c r="G49" t="n">
         <v>0.004806404196833203</v>
       </c>
-      <c r="H49" t="n">
-        <v>219.0070014953613</v>
-      </c>
-      <c r="I49" t="inlineStr"/>
-      <c r="J49" t="n">
-        <v>61.88534524231837</v>
-      </c>
     </row>
     <row r="50">
       <c r="A50" s="2" t="n">
@@ -1868,13 +1594,6 @@
       <c r="G50" t="n">
         <v>-0.002940264990135111</v>
       </c>
-      <c r="H50" t="n">
-        <v>219.3120010375977</v>
-      </c>
-      <c r="I50" t="inlineStr"/>
-      <c r="J50" t="n">
-        <v>64.16589862122659</v>
-      </c>
     </row>
     <row r="51">
       <c r="A51" s="2" t="n">
@@ -1898,13 +1617,6 @@
       <c r="G51" t="n">
         <v>0.07359155565707187</v>
       </c>
-      <c r="H51" t="n">
-        <v>220.3445007324219</v>
-      </c>
-      <c r="I51" t="inlineStr"/>
-      <c r="J51" t="n">
-        <v>70.47878571225769</v>
-      </c>
     </row>
     <row r="52">
       <c r="A52" s="2" t="n">
@@ -1928,13 +1640,6 @@
       <c r="G52" t="n">
         <v>-0.02324531900421767</v>
       </c>
-      <c r="H52" t="n">
-        <v>221.7240005493164</v>
-      </c>
-      <c r="I52" t="inlineStr"/>
-      <c r="J52" t="n">
-        <v>63.44996998061109</v>
-      </c>
     </row>
     <row r="53">
       <c r="A53" s="2" t="n">
@@ -1958,15 +1663,6 @@
       <c r="G53" t="n">
         <v>0.04931794333683115</v>
       </c>
-      <c r="H53" t="n">
-        <v>223.2080001831055</v>
-      </c>
-      <c r="I53" t="n">
-        <v>222.0138006591797</v>
-      </c>
-      <c r="J53" t="n">
-        <v>70.1061450043107</v>
-      </c>
     </row>
     <row r="54">
       <c r="A54" s="2" t="n">
@@ -1990,15 +1686,6 @@
       <c r="G54" t="n">
         <v>0.01708001708984375</v>
       </c>
-      <c r="H54" t="n">
-        <v>225.2610000610352</v>
-      </c>
-      <c r="I54" t="n">
-        <v>222.0464007568359</v>
-      </c>
-      <c r="J54" t="n">
-        <v>68.65368439221952</v>
-      </c>
     </row>
     <row r="55">
       <c r="A55" s="2" t="n">
@@ -2022,15 +1709,6 @@
       <c r="G55" t="n">
         <v>0.01081521490936144</v>
       </c>
-      <c r="H55" t="n">
-        <v>227.6514991760254</v>
-      </c>
-      <c r="I55" t="n">
-        <v>222.0556005859375</v>
-      </c>
-      <c r="J55" t="n">
-        <v>65.71461895258915</v>
-      </c>
     </row>
     <row r="56">
       <c r="A56" s="2" t="n">
@@ -2054,15 +1732,6 @@
       <c r="G56" t="n">
         <v>-0.01089404681602335</v>
       </c>
-      <c r="H56" t="n">
-        <v>230.0749992370606</v>
-      </c>
-      <c r="I56" t="n">
-        <v>222.1700006103516</v>
-      </c>
-      <c r="J56" t="n">
-        <v>81.61072033102208</v>
-      </c>
     </row>
     <row r="57">
       <c r="A57" s="2" t="n">
@@ -2086,15 +1755,6 @@
       <c r="G57" t="n">
         <v>0.02454563057356651</v>
       </c>
-      <c r="H57" t="n">
-        <v>232.7839988708496</v>
-      </c>
-      <c r="I57" t="n">
-        <v>222.3946005249023</v>
-      </c>
-      <c r="J57" t="n">
-        <v>81.79595805355754</v>
-      </c>
     </row>
     <row r="58">
       <c r="A58" s="2" t="n">
@@ -2118,15 +1778,6 @@
       <c r="G58" t="n">
         <v>0.004492104223754234</v>
       </c>
-      <c r="H58" t="n">
-        <v>235.1599990844726</v>
-      </c>
-      <c r="I58" t="n">
-        <v>222.8432006835938</v>
-      </c>
-      <c r="J58" t="n">
-        <v>79.18040464946327</v>
-      </c>
     </row>
     <row r="59">
       <c r="A59" s="2" t="n">
@@ -2150,15 +1801,6 @@
       <c r="G59" t="n">
         <v>-0.01379817223470836</v>
       </c>
-      <c r="H59" t="n">
-        <v>237.5309982299805</v>
-      </c>
-      <c r="I59" t="n">
-        <v>222.9734005737305</v>
-      </c>
-      <c r="J59" t="n">
-        <v>73.94648052614851</v>
-      </c>
     </row>
     <row r="60">
       <c r="A60" s="2" t="n">
@@ -2182,15 +1824,6 @@
       <c r="G60" t="n">
         <v>-0.03488095932262847</v>
       </c>
-      <c r="H60" t="n">
-        <v>239.0114982604981</v>
-      </c>
-      <c r="I60" t="n">
-        <v>223.0262005615234</v>
-      </c>
-      <c r="J60" t="n">
-        <v>63.77457070000304</v>
-      </c>
     </row>
     <row r="61">
       <c r="A61" s="2" t="n">
@@ -2214,15 +1847,6 @@
       <c r="G61" t="n">
         <v>-0.03357160254966751</v>
       </c>
-      <c r="H61" t="n">
-        <v>239.5359985351562</v>
-      </c>
-      <c r="I61" t="n">
-        <v>223.5196005249023</v>
-      </c>
-      <c r="J61" t="n">
-        <v>56.68084935709965</v>
-      </c>
     </row>
     <row r="62">
       <c r="A62" s="2" t="n">
@@ -2246,15 +1870,6 @@
       <c r="G62" t="n">
         <v>0.03914235030998814</v>
       </c>
-      <c r="H62" t="n">
-        <v>241.503498840332</v>
-      </c>
-      <c r="I62" t="n">
-        <v>224.1162005615234</v>
-      </c>
-      <c r="J62" t="n">
-        <v>63.9487609994583</v>
-      </c>
     </row>
     <row r="63">
       <c r="A63" s="2" t="n">
@@ -2278,15 +1893,6 @@
       <c r="G63" t="n">
         <v>-0.03698816351676526</v>
       </c>
-      <c r="H63" t="n">
-        <v>242.7314987182617</v>
-      </c>
-      <c r="I63" t="n">
-        <v>224.5368005371094</v>
-      </c>
-      <c r="J63" t="n">
-        <v>57.06806822983856</v>
-      </c>
     </row>
     <row r="64">
       <c r="A64" s="2" t="n">
@@ -2310,15 +1916,6 @@
       <c r="G64" t="n">
         <v>0.01523895752622995</v>
       </c>
-      <c r="H64" t="n">
-        <v>243.6479988098145</v>
-      </c>
-      <c r="I64" t="n">
-        <v>224.7848004150391</v>
-      </c>
-      <c r="J64" t="n">
-        <v>59.13604096860135</v>
-      </c>
     </row>
     <row r="65">
       <c r="A65" s="2" t="n">
@@ -2342,15 +1939,6 @@
       <c r="G65" t="n">
         <v>-0.01411041696622573</v>
       </c>
-      <c r="H65" t="n">
-        <v>244.2939987182617</v>
-      </c>
-      <c r="I65" t="n">
-        <v>225.1534005737305</v>
-      </c>
-      <c r="J65" t="n">
-        <v>48.23731970031961</v>
-      </c>
     </row>
     <row r="66">
       <c r="A66" s="2" t="n">
@@ -2374,15 +1962,6 @@
       <c r="G66" t="n">
         <v>-0.009458613360014412</v>
       </c>
-      <c r="H66" t="n">
-        <v>244.7419990539551</v>
-      </c>
-      <c r="I66" t="n">
-        <v>225.2874005126953</v>
-      </c>
-      <c r="J66" t="n">
-        <v>50.33325073531469</v>
-      </c>
     </row>
     <row r="67">
       <c r="A67" s="2" t="n">
@@ -2406,15 +1985,6 @@
       <c r="G67" t="n">
         <v>-0.08782510719719305</v>
       </c>
-      <c r="H67" t="n">
-        <v>244.1174995422363</v>
-      </c>
-      <c r="I67" t="n">
-        <v>225.3062005615234</v>
-      </c>
-      <c r="J67" t="n">
-        <v>31.54515922473995</v>
-      </c>
     </row>
     <row r="68">
       <c r="A68" s="2" t="n">
@@ -2438,15 +2008,6 @@
       <c r="G68" t="n">
         <v>0.00624426350457119</v>
       </c>
-      <c r="H68" t="n">
-        <v>243.736499786377</v>
-      </c>
-      <c r="I68" t="n">
-        <v>225.5360006713867</v>
-      </c>
-      <c r="J68" t="n">
-        <v>29.1829642157481</v>
-      </c>
     </row>
     <row r="69">
       <c r="A69" s="2" t="n">
@@ -2470,15 +2031,6 @@
       <c r="G69" t="n">
         <v>0.001870796017787502</v>
       </c>
-      <c r="H69" t="n">
-        <v>243.3215003967285</v>
-      </c>
-      <c r="I69" t="n">
-        <v>225.9498007202149</v>
-      </c>
-      <c r="J69" t="n">
-        <v>27.16185745211133</v>
-      </c>
     </row>
     <row r="70">
       <c r="A70" s="2" t="n">
@@ -2502,15 +2054,6 @@
       <c r="G70" t="n">
         <v>0.008015641700267029</v>
       </c>
-      <c r="H70" t="n">
-        <v>243.0280006408692</v>
-      </c>
-      <c r="I70" t="n">
-        <v>226.363600769043</v>
-      </c>
-      <c r="J70" t="n">
-        <v>29.68499034615304</v>
-      </c>
     </row>
     <row r="71">
       <c r="A71" s="2" t="n">
@@ -2534,15 +2077,6 @@
       <c r="G71" t="n">
         <v>-0.001987992760882462</v>
       </c>
-      <c r="H71" t="n">
-        <v>241.8765007019043</v>
-      </c>
-      <c r="I71" t="n">
-        <v>226.9462008666992</v>
-      </c>
-      <c r="J71" t="n">
-        <v>23.67266317714548</v>
-      </c>
     </row>
     <row r="72">
       <c r="A72" s="2" t="n">
@@ -2566,15 +2100,6 @@
       <c r="G72" t="n">
         <v>-0.0008601676940163117</v>
       </c>
-      <c r="H72" t="n">
-        <v>240.9990005493164</v>
-      </c>
-      <c r="I72" t="n">
-        <v>227.3834008789063</v>
-      </c>
-      <c r="J72" t="n">
-        <v>22.40797563366561</v>
-      </c>
     </row>
     <row r="73">
       <c r="A73" s="2" t="n">
@@ -2598,15 +2123,6 @@
       <c r="G73" t="n">
         <v>-0.008382378207102636</v>
       </c>
-      <c r="H73" t="n">
-        <v>239.4415008544922</v>
-      </c>
-      <c r="I73" t="n">
-        <v>227.7604010009766</v>
-      </c>
-      <c r="J73" t="n">
-        <v>22.95263262149507</v>
-      </c>
     </row>
     <row r="74">
       <c r="A74" s="2" t="n">
@@ -2630,15 +2146,6 @@
       <c r="G74" t="n">
         <v>-0.004021041161846095</v>
       </c>
-      <c r="H74" t="n">
-        <v>237.6265007019043</v>
-      </c>
-      <c r="I74" t="n">
-        <v>228.1700009155273</v>
-      </c>
-      <c r="J74" t="n">
-        <v>25.85160499740229</v>
-      </c>
     </row>
     <row r="75">
       <c r="A75" s="2" t="n">
@@ -2662,15 +2169,6 @@
       <c r="G75" t="n">
         <v>-0.01981927467094236</v>
       </c>
-      <c r="H75" t="n">
-        <v>235.4580009460449</v>
-      </c>
-      <c r="I75" t="n">
-        <v>228.2864007568359</v>
-      </c>
-      <c r="J75" t="n">
-        <v>27.58505413641079</v>
-      </c>
     </row>
     <row r="76">
       <c r="A76" s="2" t="n">
@@ -2694,15 +2192,6 @@
       <c r="G76" t="n">
         <v>0.2191903507029043</v>
       </c>
-      <c r="H76" t="n">
-        <v>235.7710014343262</v>
-      </c>
-      <c r="I76" t="n">
-        <v>229.4684008789062</v>
-      </c>
-      <c r="J76" t="n">
-        <v>55.32459919124996</v>
-      </c>
     </row>
     <row r="77">
       <c r="A77" s="2" t="n">
@@ -2726,15 +2215,6 @@
       <c r="G77" t="n">
         <v>0.03343823359841336</v>
       </c>
-      <c r="H77" t="n">
-        <v>236.2075019836426</v>
-      </c>
-      <c r="I77" t="n">
-        <v>230.5694009399414</v>
-      </c>
-      <c r="J77" t="n">
-        <v>64.60049298829495</v>
-      </c>
     </row>
     <row r="78">
       <c r="A78" s="2" t="n">
@@ -2758,15 +2238,6 @@
       <c r="G78" t="n">
         <v>-0.02481515886621855</v>
       </c>
-      <c r="H78" t="n">
-        <v>236.2515022277832</v>
-      </c>
-      <c r="I78" t="n">
-        <v>231.4972012329102</v>
-      </c>
-      <c r="J78" t="n">
-        <v>58.99331313660829</v>
-      </c>
     </row>
     <row r="79">
       <c r="A79" s="2" t="n">
@@ -2790,15 +2261,6 @@
       <c r="G79" t="n">
         <v>-0.01139012091242797</v>
       </c>
-      <c r="H79" t="n">
-        <v>236.3265022277832</v>
-      </c>
-      <c r="I79" t="n">
-        <v>232.2332009887695</v>
-      </c>
-      <c r="J79" t="n">
-        <v>59.26556669307521</v>
-      </c>
     </row>
     <row r="80">
       <c r="A80" s="2" t="n">
@@ -2822,15 +2284,6 @@
       <c r="G80" t="n">
         <v>-0.007590942139718337</v>
       </c>
-      <c r="H80" t="n">
-        <v>236.7530014038086</v>
-      </c>
-      <c r="I80" t="n">
-        <v>232.9622006225586</v>
-      </c>
-      <c r="J80" t="n">
-        <v>59.45047183828269</v>
-      </c>
     </row>
     <row r="81">
       <c r="A81" s="2" t="n">
@@ -2854,15 +2307,6 @@
       <c r="G81" t="n">
         <v>-0.02989703767970175</v>
       </c>
-      <c r="H81" t="n">
-        <v>237.2125015258789</v>
-      </c>
-      <c r="I81" t="n">
-        <v>233.4938006591797</v>
-      </c>
-      <c r="J81" t="n">
-        <v>68.61424017568254</v>
-      </c>
     </row>
     <row r="82">
       <c r="A82" s="2" t="n">
@@ -2886,15 +2330,6 @@
       <c r="G82" t="n">
         <v>-0.003482130697311625</v>
       </c>
-      <c r="H82" t="n">
-        <v>237.1575012207031</v>
-      </c>
-      <c r="I82" t="n">
-        <v>234.2602005004883</v>
-      </c>
-      <c r="J82" t="n">
-        <v>67.41821531750307</v>
-      </c>
     </row>
     <row r="83">
       <c r="A83" s="2" t="n">
@@ -2918,15 +2353,6 @@
       <c r="G83" t="n">
         <v>-0.02466061328223124</v>
       </c>
-      <c r="H83" t="n">
-        <v>237.2580009460449</v>
-      </c>
-      <c r="I83" t="n">
-        <v>234.7106002807617</v>
-      </c>
-      <c r="J83" t="n">
-        <v>62.73950764225773</v>
-      </c>
     </row>
     <row r="84">
       <c r="A84" s="2" t="n">
@@ -2950,15 +2376,6 @@
       <c r="G84" t="n">
         <v>0.03541429020427711</v>
       </c>
-      <c r="H84" t="n">
-        <v>237.6050010681152</v>
-      </c>
-      <c r="I84" t="n">
-        <v>235.4752001953125</v>
-      </c>
-      <c r="J84" t="n">
-        <v>65.33563808283016</v>
-      </c>
     </row>
     <row r="85">
       <c r="A85" s="2" t="n">
@@ -2982,15 +2399,6 @@
       <c r="G85" t="n">
         <v>0.1475103244422447</v>
       </c>
-      <c r="H85" t="n">
-        <v>239.9790008544922</v>
-      </c>
-      <c r="I85" t="n">
-        <v>237.0616000366211</v>
-      </c>
-      <c r="J85" t="n">
-        <v>75.08529448880745</v>
-      </c>
     </row>
     <row r="86">
       <c r="A86" s="2" t="n">
@@ -3014,15 +2422,6 @@
       <c r="G86" t="n">
         <v>0.02904379065700735</v>
       </c>
-      <c r="H86" t="n">
-        <v>242.8860008239746</v>
-      </c>
-      <c r="I86" t="n">
-        <v>238.8848001098633</v>
-      </c>
-      <c r="J86" t="n">
-        <v>76.64498754575315</v>
-      </c>
     </row>
     <row r="87">
       <c r="A87" s="2" t="n">
@@ -3046,15 +2445,6 @@
       <c r="G87" t="n">
         <v>0.08187665372925301</v>
       </c>
-      <c r="H87" t="n">
-        <v>248.0570007324219</v>
-      </c>
-      <c r="I87" t="n">
-        <v>241.1836001586914</v>
-      </c>
-      <c r="J87" t="n">
-        <v>80.93309224690998</v>
-      </c>
     </row>
     <row r="88">
       <c r="A88" s="2" t="n">
@@ -3078,15 +2468,6 @@
       <c r="G88" t="n">
         <v>0.08959591143118995</v>
       </c>
-      <c r="H88" t="n">
-        <v>254.5990005493164</v>
-      </c>
-      <c r="I88" t="n">
-        <v>243.9014001464844</v>
-      </c>
-      <c r="J88" t="n">
-        <v>84.1392101350478</v>
-      </c>
     </row>
     <row r="89">
       <c r="A89" s="2" t="n">
@@ -3110,15 +2491,6 @@
       <c r="G89" t="n">
         <v>-0.06145717075892854</v>
       </c>
-      <c r="H89" t="n">
-        <v>260.0449996948242</v>
-      </c>
-      <c r="I89" t="n">
-        <v>246.2591998291016</v>
-      </c>
-      <c r="J89" t="n">
-        <v>77.27013227229108</v>
-      </c>
     </row>
     <row r="90">
       <c r="A90" s="2" t="n">
@@ -3142,15 +2514,6 @@
       <c r="G90" t="n">
         <v>0.005327407385385952</v>
       </c>
-      <c r="H90" t="n">
-        <v>265.4904991149903</v>
-      </c>
-      <c r="I90" t="n">
-        <v>248.4757995605469</v>
-      </c>
-      <c r="J90" t="n">
-        <v>71.07806823079387</v>
-      </c>
     </row>
     <row r="91">
       <c r="A91" s="2" t="n">
@@ -3174,15 +2537,6 @@
       <c r="G91" t="n">
         <v>-0.05771559508909463</v>
       </c>
-      <c r="H91" t="n">
-        <v>270.0049987792969</v>
-      </c>
-      <c r="I91" t="n">
-        <v>250.0959994506836</v>
-      </c>
-      <c r="J91" t="n">
-        <v>61.94050678301402</v>
-      </c>
     </row>
     <row r="92">
       <c r="A92" s="2" t="n">
@@ -3206,15 +2560,6 @@
       <c r="G92" t="n">
         <v>0.03065752544978562</v>
       </c>
-      <c r="H92" t="n">
-        <v>275.0059989929199</v>
-      </c>
-      <c r="I92" t="n">
-        <v>252.2957995605469</v>
-      </c>
-      <c r="J92" t="n">
-        <v>66.28797938283422</v>
-      </c>
     </row>
     <row r="93">
       <c r="A93" s="2" t="n">
@@ -3238,15 +2583,6 @@
       <c r="G93" t="n">
         <v>0.05618604684798378</v>
       </c>
-      <c r="H93" t="n">
-        <v>281.0004981994629</v>
-      </c>
-      <c r="I93" t="n">
-        <v>254.7451992797852</v>
-      </c>
-      <c r="J93" t="n">
-        <v>70.44703714678606</v>
-      </c>
     </row>
     <row r="94">
       <c r="A94" s="2" t="n">
@@ -3270,15 +2606,6 @@
       <c r="G94" t="n">
         <v>0.02143239645428863</v>
       </c>
-      <c r="H94" t="n">
-        <v>287.4019981384278</v>
-      </c>
-      <c r="I94" t="n">
-        <v>257.1417993164063</v>
-      </c>
-      <c r="J94" t="n">
-        <v>72.22250335829821</v>
-      </c>
     </row>
     <row r="95">
       <c r="A95" s="2" t="n">
@@ -3302,15 +2629,6 @@
       <c r="G95" t="n">
         <v>-0.01147399196735011</v>
       </c>
-      <c r="H95" t="n">
-        <v>293.8209983825683</v>
-      </c>
-      <c r="I95" t="n">
-        <v>259.419799194336</v>
-      </c>
-      <c r="J95" t="n">
-        <v>73.60200195782549</v>
-      </c>
     </row>
     <row r="96">
       <c r="A96" s="2" t="n">
@@ -3334,15 +2652,6 @@
       <c r="G96" t="n">
         <v>-0.006987644766217049</v>
       </c>
-      <c r="H96" t="n">
-        <v>297.7789985656738</v>
-      </c>
-      <c r="I96" t="n">
-        <v>261.6163995361328</v>
-      </c>
-      <c r="J96" t="n">
-        <v>73.03354103532588</v>
-      </c>
     </row>
     <row r="97">
       <c r="A97" s="2" t="n">
@@ -3366,15 +2675,6 @@
       <c r="G97" t="n">
         <v>0.03804022598317736</v>
       </c>
-      <c r="H97" t="n">
-        <v>301.9474983215332</v>
-      </c>
-      <c r="I97" t="n">
-        <v>264.0617996215821</v>
-      </c>
-      <c r="J97" t="n">
-        <v>76.9476393696871</v>
-      </c>
     </row>
     <row r="98">
       <c r="A98" s="2" t="n">
@@ -3398,15 +2698,6 @@
       <c r="G98" t="n">
         <v>-0.03962446482142767</v>
       </c>
-      <c r="H98" t="n">
-        <v>305.7514976501465</v>
-      </c>
-      <c r="I98" t="n">
-        <v>266.2979995727539</v>
-      </c>
-      <c r="J98" t="n">
-        <v>70.85427172374892</v>
-      </c>
     </row>
     <row r="99">
       <c r="A99" s="2" t="n">
@@ -3430,15 +2721,6 @@
       <c r="G99" t="n">
         <v>-0.001063189566898104</v>
       </c>
-      <c r="H99" t="n">
-        <v>309.6869987487793</v>
-      </c>
-      <c r="I99" t="n">
-        <v>268.5051998901367</v>
-      </c>
-      <c r="J99" t="n">
-        <v>64.42922444015066</v>
-      </c>
     </row>
     <row r="100">
       <c r="A100" s="2" t="n">
@@ -3462,15 +2744,6 @@
       <c r="G100" t="n">
         <v>-0.01578806186452353</v>
       </c>
-      <c r="H100" t="n">
-        <v>313.4540000915528</v>
-      </c>
-      <c r="I100" t="n">
-        <v>270.6190002441406</v>
-      </c>
-      <c r="J100" t="n">
-        <v>60.63365026429152</v>
-      </c>
     </row>
     <row r="101">
       <c r="A101" s="2" t="n">
@@ -3494,15 +2767,6 @@
       <c r="G101" t="n">
         <v>0.03685898787510977</v>
       </c>
-      <c r="H101" t="n">
-        <v>318.2194999694824</v>
-      </c>
-      <c r="I101" t="n">
-        <v>272.6438003540039</v>
-      </c>
-      <c r="J101" t="n">
-        <v>57.61741425109561</v>
-      </c>
     </row>
     <row r="102">
       <c r="A102" s="2" t="n">
@@ -3526,15 +2790,6 @@
       <c r="G102" t="n">
         <v>0.03456365902539504</v>
       </c>
-      <c r="H102" t="n">
-        <v>323.625</v>
-      </c>
-      <c r="I102" t="n">
-        <v>275.0206002807617</v>
-      </c>
-      <c r="J102" t="n">
-        <v>52.52690818684535</v>
-      </c>
     </row>
     <row r="103">
       <c r="A103" s="2" t="n">
@@ -3558,15 +2813,6 @@
       <c r="G103" t="n">
         <v>-0.01587830229999254</v>
       </c>
-      <c r="H103" t="n">
-        <v>329.0540008544922</v>
-      </c>
-      <c r="I103" t="n">
-        <v>277.0490005493164</v>
-      </c>
-      <c r="J103" t="n">
-        <v>59.21255034667942</v>
-      </c>
     </row>
     <row r="104">
       <c r="A104" s="2" t="n">
@@ -3590,15 +2836,6 @@
       <c r="G104" t="n">
         <v>0.01852478230977472</v>
       </c>
-      <c r="H104" t="n">
-        <v>334.3785003662109</v>
-      </c>
-      <c r="I104" t="n">
-        <v>279.1222003173828</v>
-      </c>
-      <c r="J104" t="n">
-        <v>60.71512417482493</v>
-      </c>
     </row>
     <row r="105">
       <c r="A105" s="2" t="n">
@@ -3622,15 +2859,6 @@
       <c r="G105" t="n">
         <v>0.03229681165351517</v>
       </c>
-      <c r="H105" t="n">
-        <v>338.4264999389649</v>
-      </c>
-      <c r="I105" t="n">
-        <v>281.3716003417969</v>
-      </c>
-      <c r="J105" t="n">
-        <v>73.95450066320812</v>
-      </c>
     </row>
     <row r="106">
       <c r="A106" s="2" t="n">
@@ -3654,15 +2882,6 @@
       <c r="G106" t="n">
         <v>0.053397958017247</v>
       </c>
-      <c r="H106" t="n">
-        <v>343.0419998168945</v>
-      </c>
-      <c r="I106" t="n">
-        <v>284.0716003417969</v>
-      </c>
-      <c r="J106" t="n">
-        <v>75.9666606202176</v>
-      </c>
     </row>
     <row r="107">
       <c r="A107" s="2" t="n">
@@ -3686,15 +2905,6 @@
       <c r="G107" t="n">
         <v>0.001464486209421523</v>
       </c>
-      <c r="H107" t="n">
-        <v>346.4705001831055</v>
-      </c>
-      <c r="I107" t="n">
-        <v>286.6582006835937</v>
-      </c>
-      <c r="J107" t="n">
-        <v>72.30233888267456</v>
-      </c>
     </row>
     <row r="108">
       <c r="A108" s="2" t="n">
@@ -3718,15 +2928,6 @@
       <c r="G108" t="n">
         <v>0.02873337295448497</v>
       </c>
-      <c r="H108" t="n">
-        <v>349.0199996948242</v>
-      </c>
-      <c r="I108" t="n">
-        <v>289.445400390625</v>
-      </c>
-      <c r="J108" t="n">
-        <v>73.22410682064236</v>
-      </c>
     </row>
     <row r="109">
       <c r="A109" s="2" t="n">
@@ -3750,15 +2951,6 @@
       <c r="G109" t="n">
         <v>0.05930322291934931</v>
       </c>
-      <c r="H109" t="n">
-        <v>353.8339996337891</v>
-      </c>
-      <c r="I109" t="n">
-        <v>292.780400390625</v>
-      </c>
-      <c r="J109" t="n">
-        <v>79.93489725372493</v>
-      </c>
     </row>
     <row r="110">
       <c r="A110" s="2" t="n">
@@ -3782,15 +2974,6 @@
       <c r="G110" t="n">
         <v>-0.01570257570607603</v>
       </c>
-      <c r="H110" t="n">
-        <v>358.2270004272461</v>
-      </c>
-      <c r="I110" t="n">
-        <v>296.1620004272461</v>
-      </c>
-      <c r="J110" t="n">
-        <v>77.53370740670852</v>
-      </c>
     </row>
     <row r="111">
       <c r="A111" s="2" t="n">
@@ -3814,15 +2997,6 @@
       <c r="G111" t="n">
         <v>0.04336284290396253</v>
       </c>
-      <c r="H111" t="n">
-        <v>364.4795013427735</v>
-      </c>
-      <c r="I111" t="n">
-        <v>300.0734005737305</v>
-      </c>
-      <c r="J111" t="n">
-        <v>78.3262454842987</v>
-      </c>
     </row>
     <row r="112">
       <c r="A112" s="2" t="n">
@@ -3846,15 +3020,6 @@
       <c r="G112" t="n">
         <v>0.06141250567967771</v>
       </c>
-      <c r="H112" t="n">
-        <v>371.5945007324219</v>
-      </c>
-      <c r="I112" t="n">
-        <v>304.3322003173828</v>
-      </c>
-      <c r="J112" t="n">
-        <v>88.76084970914071</v>
-      </c>
     </row>
     <row r="113">
       <c r="A113" s="2" t="n">
@@ -3878,15 +3043,6 @@
       <c r="G113" t="n">
         <v>0.03636991217973828</v>
       </c>
-      <c r="H113" t="n">
-        <v>378.6505004882812</v>
-      </c>
-      <c r="I113" t="n">
-        <v>309.112799987793</v>
-      </c>
-      <c r="J113" t="n">
-        <v>90.01075073216194</v>
-      </c>
     </row>
     <row r="114">
       <c r="A114" s="2" t="n">
@@ -3910,15 +3066,6 @@
       <c r="G114" t="n">
         <v>-0.08279494369517471</v>
       </c>
-      <c r="H114" t="n">
-        <v>383.3570007324219</v>
-      </c>
-      <c r="I114" t="n">
-        <v>313.0254000854492</v>
-      </c>
-      <c r="J114" t="n">
-        <v>75.36665003488056</v>
-      </c>
     </row>
     <row r="115">
       <c r="A115" s="2" t="n">
@@ -3942,15 +3089,6 @@
       <c r="G115" t="n">
         <v>-0.008997322180141931</v>
       </c>
-      <c r="H115" t="n">
-        <v>388.0640014648437</v>
-      </c>
-      <c r="I115" t="n">
-        <v>316.9278002929688</v>
-      </c>
-      <c r="J115" t="n">
-        <v>72.40854414524134</v>
-      </c>
     </row>
     <row r="116">
       <c r="A116" s="2" t="n">
@@ -3974,15 +3112,6 @@
       <c r="G116" t="n">
         <v>-0.03464249123958651</v>
       </c>
-      <c r="H116" t="n">
-        <v>392.1350006103515</v>
-      </c>
-      <c r="I116" t="n">
-        <v>320.5736001586914</v>
-      </c>
-      <c r="J116" t="n">
-        <v>65.50788596763405</v>
-      </c>
     </row>
     <row r="117">
       <c r="A117" s="2" t="n">
@@ -4006,15 +3135,6 @@
       <c r="G117" t="n">
         <v>0.02265712392589436</v>
       </c>
-      <c r="H117" t="n">
-        <v>396.0370010375976</v>
-      </c>
-      <c r="I117" t="n">
-        <v>324.8296002197266</v>
-      </c>
-      <c r="J117" t="n">
-        <v>68.84161848367734</v>
-      </c>
     </row>
     <row r="118">
       <c r="A118" s="2" t="n">
@@ -4038,15 +3158,6 @@
       <c r="G118" t="n">
         <v>0.07357174228224572</v>
       </c>
-      <c r="H118" t="n">
-        <v>402.221501159668</v>
-      </c>
-      <c r="I118" t="n">
-        <v>329.6920001220703</v>
-      </c>
-      <c r="J118" t="n">
-        <v>72.17476930228491</v>
-      </c>
     </row>
     <row r="119">
       <c r="A119" s="2" t="n">
@@ -4070,15 +3181,6 @@
       <c r="G119" t="n">
         <v>-0.01762999463097115</v>
       </c>
-      <c r="H119" t="n">
-        <v>408.0165008544922</v>
-      </c>
-      <c r="I119" t="n">
-        <v>334.3832000732422</v>
-      </c>
-      <c r="J119" t="n">
-        <v>68.25082696760646</v>
-      </c>
     </row>
     <row r="120">
       <c r="A120" s="2" t="n">
@@ -4102,15 +3204,6 @@
       <c r="G120" t="n">
         <v>-0.04947922616674816</v>
       </c>
-      <c r="H120" t="n">
-        <v>412.9550003051758</v>
-      </c>
-      <c r="I120" t="n">
-        <v>338.5898001098633</v>
-      </c>
-      <c r="J120" t="n">
-        <v>59.04441530244565</v>
-      </c>
     </row>
     <row r="121">
       <c r="A121" s="2" t="n">
@@ -4134,15 +3227,6 @@
       <c r="G121" t="n">
         <v>-0.03301209257078741</v>
       </c>
-      <c r="H121" t="n">
-        <v>416.5675003051758</v>
-      </c>
-      <c r="I121" t="n">
-        <v>342.5202001953125</v>
-      </c>
-      <c r="J121" t="n">
-        <v>55.56182103592152</v>
-      </c>
     </row>
     <row r="122">
       <c r="A122" s="2" t="n">
@@ -4166,15 +3250,6 @@
       <c r="G122" t="n">
         <v>-0.03251001941775111</v>
       </c>
-      <c r="H122" t="n">
-        <v>418.9050003051758</v>
-      </c>
-      <c r="I122" t="n">
-        <v>346.1830001831055</v>
-      </c>
-      <c r="J122" t="n">
-        <v>50.56847780843158</v>
-      </c>
     </row>
     <row r="123">
       <c r="A123" s="2" t="n">
@@ -4198,15 +3273,6 @@
       <c r="G123" t="n">
         <v>-0.06081615932376483</v>
       </c>
-      <c r="H123" t="n">
-        <v>420.2979995727539</v>
-      </c>
-      <c r="I123" t="n">
-        <v>349.3916000366211</v>
-      </c>
-      <c r="J123" t="n">
-        <v>40.95446429351641</v>
-      </c>
     </row>
     <row r="124">
       <c r="A124" s="2" t="n">
@@ -4230,15 +3296,6 @@
       <c r="G124" t="n">
         <v>0.08215567328200035</v>
       </c>
-      <c r="H124" t="n">
-        <v>422.9235000610352</v>
-      </c>
-      <c r="I124" t="n">
-        <v>353.2410000610352</v>
-      </c>
-      <c r="J124" t="n">
-        <v>48.61201630037421</v>
-      </c>
     </row>
     <row r="125">
       <c r="A125" s="2" t="n">
@@ -4262,15 +3319,6 @@
       <c r="G125" t="n">
         <v>0.00148617422262487</v>
       </c>
-      <c r="H125" t="n">
-        <v>425.0014999389649</v>
-      </c>
-      <c r="I125" t="n">
-        <v>357.1889999389649</v>
-      </c>
-      <c r="J125" t="n">
-        <v>45.12808067638927</v>
-      </c>
     </row>
     <row r="126">
       <c r="A126" s="2" t="n">
@@ -4294,15 +3342,6 @@
       <c r="G126" t="n">
         <v>-0.0406033400731115</v>
       </c>
-      <c r="H126" t="n">
-        <v>425.2584991455078</v>
-      </c>
-      <c r="I126" t="n">
-        <v>359.8665994262695</v>
-      </c>
-      <c r="J126" t="n">
-        <v>36.17509462084621</v>
-      </c>
     </row>
     <row r="127">
       <c r="A127" s="2" t="n">
@@ -4326,15 +3365,6 @@
       <c r="G127" t="n">
         <v>0.001470780787575787</v>
       </c>
-      <c r="H127" t="n">
-        <v>425.515998840332</v>
-      </c>
-      <c r="I127" t="n">
-        <v>362.3815994262695</v>
-      </c>
-      <c r="J127" t="n">
-        <v>31.703011332508</v>
-      </c>
     </row>
     <row r="128">
       <c r="A128" s="2" t="n">
@@ -4358,15 +3388,6 @@
       <c r="G128" t="n">
         <v>-0.0005064369418008585</v>
       </c>
-      <c r="H128" t="n">
-        <v>425.203498840332</v>
-      </c>
-      <c r="I128" t="n">
-        <v>365.0261990356445</v>
-      </c>
-      <c r="J128" t="n">
-        <v>38.21222465549839</v>
-      </c>
     </row>
     <row r="129">
       <c r="A129" s="2" t="n">
@@ -4390,15 +3411,6 @@
       <c r="G129" t="n">
         <v>0.02171051207436658</v>
       </c>
-      <c r="H129" t="n">
-        <v>424.1304992675781</v>
-      </c>
-      <c r="I129" t="n">
-        <v>367.901999206543</v>
-      </c>
-      <c r="J129" t="n">
-        <v>41.66581912835909</v>
-      </c>
     </row>
     <row r="130">
       <c r="A130" s="2" t="n">
@@ -4422,15 +3434,6 @@
       <c r="G130" t="n">
         <v>-0.01723243224592153</v>
       </c>
-      <c r="H130" t="n">
-        <v>423.0434982299805</v>
-      </c>
-      <c r="I130" t="n">
-        <v>370.6781991577149</v>
-      </c>
-      <c r="J130" t="n">
-        <v>43.46491512794998</v>
-      </c>
     </row>
     <row r="131">
       <c r="A131" s="2" t="n">
@@ -4454,15 +3457,6 @@
       <c r="G131" t="n">
         <v>0.08038151439752794</v>
       </c>
-      <c r="H131" t="n">
-        <v>422.6429977416992</v>
-      </c>
-      <c r="I131" t="n">
-        <v>374.2455990600586</v>
-      </c>
-      <c r="J131" t="n">
-        <v>49.43681866236849</v>
-      </c>
     </row>
     <row r="132">
       <c r="A132" s="2" t="n">
@@ -4486,15 +3480,6 @@
       <c r="G132" t="n">
         <v>-0.03362756026209679</v>
       </c>
-      <c r="H132" t="n">
-        <v>420.1829986572266</v>
-      </c>
-      <c r="I132" t="n">
-        <v>377.5423992919922</v>
-      </c>
-      <c r="J132" t="n">
-        <v>37.51160216614664</v>
-      </c>
     </row>
     <row r="133">
       <c r="A133" s="2" t="n">
@@ -4518,15 +3503,6 @@
       <c r="G133" t="n">
         <v>0.03064132340475934</v>
       </c>
-      <c r="H133" t="n">
-        <v>417.5149993896484</v>
-      </c>
-      <c r="I133" t="n">
-        <v>381.2155993652344</v>
-      </c>
-      <c r="J133" t="n">
-        <v>43.0420553795153</v>
-      </c>
     </row>
     <row r="134">
       <c r="A134" s="2" t="n">
@@ -4550,15 +3526,6 @@
       <c r="G134" t="n">
         <v>-0.00569752092797482</v>
       </c>
-      <c r="H134" t="n">
-        <v>416.7119995117188</v>
-      </c>
-      <c r="I134" t="n">
-        <v>384.6681994628906</v>
-      </c>
-      <c r="J134" t="n">
-        <v>47.87407018511417</v>
-      </c>
     </row>
     <row r="135">
       <c r="A135" s="2" t="n">
@@ -4582,15 +3549,6 @@
       <c r="G135" t="n">
         <v>-0.0211286387103673</v>
       </c>
-      <c r="H135" t="n">
-        <v>415.6589981079102</v>
-      </c>
-      <c r="I135" t="n">
-        <v>387.1997991943359</v>
-      </c>
-      <c r="J135" t="n">
-        <v>49.33609932920196</v>
-      </c>
     </row>
     <row r="136">
       <c r="A136" s="2" t="n">
@@ -4614,15 +3572,6 @@
       <c r="G136" t="n">
         <v>-0.006576523247056931</v>
       </c>
-      <c r="H136" t="n">
-        <v>415.2249984741211</v>
-      </c>
-      <c r="I136" t="n">
-        <v>389.50919921875</v>
-      </c>
-      <c r="J136" t="n">
-        <v>52.6296362492668</v>
-      </c>
     </row>
     <row r="137">
       <c r="A137" s="2" t="n">
@@ -4646,15 +3595,6 @@
       <c r="G137" t="n">
         <v>-0.01406474184458839</v>
       </c>
-      <c r="H137" t="n">
-        <v>414.0239974975586</v>
-      </c>
-      <c r="I137" t="n">
-        <v>391.2163989257813</v>
-      </c>
-      <c r="J137" t="n">
-        <v>59.50423935359366</v>
-      </c>
     </row>
     <row r="138">
       <c r="A138" s="2" t="n">
@@ -4678,15 +3618,6 @@
       <c r="G138" t="n">
         <v>-0.02319345021205355</v>
       </c>
-      <c r="H138" t="n">
-        <v>410.767497253418</v>
-      </c>
-      <c r="I138" t="n">
-        <v>392.1593988037109</v>
-      </c>
-      <c r="J138" t="n">
-        <v>44.54836179327823</v>
-      </c>
     </row>
     <row r="139">
       <c r="A139" s="2" t="n">
@@ -4710,15 +3641,6 @@
       <c r="G139" t="n">
         <v>0.002366870089015372</v>
       </c>
-      <c r="H139" t="n">
-        <v>407.9654968261719</v>
-      </c>
-      <c r="I139" t="n">
-        <v>393.5513989257813</v>
-      </c>
-      <c r="J139" t="n">
-        <v>44.69809161610994</v>
-      </c>
     </row>
     <row r="140">
       <c r="A140" s="2" t="n">
@@ -4742,15 +3664,6 @@
       <c r="G140" t="n">
         <v>-0.02258280870425211</v>
       </c>
-      <c r="H140" t="n">
-        <v>405.8374969482422</v>
-      </c>
-      <c r="I140" t="n">
-        <v>394.7285992431641</v>
-      </c>
-      <c r="J140" t="n">
-        <v>47.70346797534398</v>
-      </c>
     </row>
     <row r="141">
       <c r="A141" s="2" t="n">
@@ -4774,15 +3687,6 @@
       <c r="G141" t="n">
         <v>0.02873295425445699</v>
       </c>
-      <c r="H141" t="n">
-        <v>404.9809967041016</v>
-      </c>
-      <c r="I141" t="n">
-        <v>396.5105993652344</v>
-      </c>
-      <c r="J141" t="n">
-        <v>52.13394950600411</v>
-      </c>
     </row>
     <row r="142">
       <c r="A142" s="2" t="n">
@@ -4806,15 +3710,6 @@
       <c r="G142" t="n">
         <v>0.01079246361894959</v>
       </c>
-      <c r="H142" t="n">
-        <v>405.0189971923828</v>
-      </c>
-      <c r="I142" t="n">
-        <v>398.1881994628906</v>
-      </c>
-      <c r="J142" t="n">
-        <v>53.81461400724498</v>
-      </c>
     </row>
     <row r="143">
       <c r="A143" s="2" t="n">
@@ -4838,15 +3733,6 @@
       <c r="G143" t="n">
         <v>-0.05170542044525339</v>
       </c>
-      <c r="H143" t="n">
-        <v>405.238996887207</v>
-      </c>
-      <c r="I143" t="n">
-        <v>399.0869995117188</v>
-      </c>
-      <c r="J143" t="n">
-        <v>43.0680128682897</v>
-      </c>
     </row>
     <row r="144">
       <c r="A144" s="2" t="n">
@@ -4870,15 +3756,6 @@
       <c r="G144" t="n">
         <v>0.02223206563315627</v>
       </c>
-      <c r="H144" t="n">
-        <v>404.3274963378906</v>
-      </c>
-      <c r="I144" t="n">
-        <v>400.0111993408203</v>
-      </c>
-      <c r="J144" t="n">
-        <v>48.55067629138028</v>
-      </c>
     </row>
     <row r="145">
       <c r="A145" s="2" t="n">
@@ -4902,15 +3779,6 @@
       <c r="G145" t="n">
         <v>-0.03579709424345923</v>
       </c>
-      <c r="H145" t="n">
-        <v>402.6834976196289</v>
-      </c>
-      <c r="I145" t="n">
-        <v>400.733999633789</v>
-      </c>
-      <c r="J145" t="n">
-        <v>30.03590046227993</v>
-      </c>
     </row>
     <row r="146">
       <c r="A146" s="2" t="n">
@@ -4934,15 +3802,6 @@
       <c r="G146" t="n">
         <v>-0.01018062238361828</v>
       </c>
-      <c r="H146" t="n">
-        <v>401.6814987182617</v>
-      </c>
-      <c r="I146" t="n">
-        <v>401.4275994873047</v>
-      </c>
-      <c r="J146" t="n">
-        <v>32.79616541805099</v>
-      </c>
     </row>
     <row r="147">
       <c r="A147" s="2" t="n">
@@ -4966,15 +3825,6 @@
       <c r="G147" t="n">
         <v>-0.0339282217314959</v>
       </c>
-      <c r="H147" t="n">
-        <v>400.0154983520508</v>
-      </c>
-      <c r="I147" t="n">
-        <v>401.6087994384766</v>
-      </c>
-      <c r="J147" t="n">
-        <v>21.74708206575446</v>
-      </c>
     </row>
     <row r="148">
       <c r="A148" s="2" t="n">
@@ -4998,15 +3848,6 @@
       <c r="G148" t="n">
         <v>-0.03011444134147045</v>
       </c>
-      <c r="H148" t="n">
-        <v>397.8149993896484</v>
-      </c>
-      <c r="I148" t="n">
-        <v>401.8515997314453</v>
-      </c>
-      <c r="J148" t="n">
-        <v>20.25470592793069</v>
-      </c>
     </row>
     <row r="149">
       <c r="A149" s="2" t="n">
@@ -5030,15 +3871,6 @@
       <c r="G149" t="n">
         <v>-0.06338211812502892</v>
       </c>
-      <c r="H149" t="n">
-        <v>394.0744995117187</v>
-      </c>
-      <c r="I149" t="n">
-        <v>401.6569995117188</v>
-      </c>
-      <c r="J149" t="n">
-        <v>18.28634452795526</v>
-      </c>
     </row>
     <row r="150">
       <c r="A150" s="2" t="n">
@@ -5062,15 +3894,6 @@
       <c r="G150" t="n">
         <v>0.0243835913717656</v>
       </c>
-      <c r="H150" t="n">
-        <v>391.0820007324219</v>
-      </c>
-      <c r="I150" t="n">
-        <v>401.7293994140625</v>
-      </c>
-      <c r="J150" t="n">
-        <v>23.25319538348261</v>
-      </c>
     </row>
     <row r="151">
       <c r="A151" s="2" t="n">
@@ -5094,15 +3917,6 @@
       <c r="G151" t="n">
         <v>0.05773971683431944</v>
       </c>
-      <c r="H151" t="n">
-        <v>387.468000793457</v>
-      </c>
-      <c r="I151" t="n">
-        <v>401.9449993896484</v>
-      </c>
-      <c r="J151" t="n">
-        <v>33.71285638932628</v>
-      </c>
     </row>
     <row r="152">
       <c r="A152" s="2" t="n">
@@ -5126,15 +3940,6 @@
       <c r="G152" t="n">
         <v>-0.0002809633725618932</v>
       </c>
-      <c r="H152" t="n">
-        <v>384.5690002441406</v>
-      </c>
-      <c r="I152" t="n">
-        <v>401.9199993896484</v>
-      </c>
-      <c r="J152" t="n">
-        <v>35.86532670284865</v>
-      </c>
     </row>
     <row r="153">
       <c r="A153" s="2" t="n">
@@ -5158,15 +3963,6 @@
       <c r="G153" t="n">
         <v>-0.004861766535893763</v>
       </c>
-      <c r="H153" t="n">
-        <v>380.9494995117187</v>
-      </c>
-      <c r="I153" t="n">
-        <v>401.973798828125</v>
-      </c>
-      <c r="J153" t="n">
-        <v>35.03266847033044</v>
-      </c>
     </row>
     <row r="154">
       <c r="A154" s="2" t="n">
@@ -5190,15 +3986,6 @@
       <c r="G154" t="n">
         <v>0.01821471428044497</v>
       </c>
-      <c r="H154" t="n">
-        <v>377.7739990234375</v>
-      </c>
-      <c r="I154" t="n">
-        <v>402.0263989257812</v>
-      </c>
-      <c r="J154" t="n">
-        <v>40.11635907077612</v>
-      </c>
     </row>
     <row r="155">
       <c r="A155" s="2" t="n">
@@ -5222,15 +4009,6 @@
       <c r="G155" t="n">
         <v>-0.01708454543992588</v>
       </c>
-      <c r="H155" t="n">
-        <v>374.7384994506836</v>
-      </c>
-      <c r="I155" t="n">
-        <v>401.7245989990234</v>
-      </c>
-      <c r="J155" t="n">
-        <v>33.53903931852274</v>
-      </c>
     </row>
     <row r="156">
       <c r="A156" s="2" t="n">
@@ -5254,15 +4032,6 @@
       <c r="G156" t="n">
         <v>-0.04683974714842765</v>
       </c>
-      <c r="H156" t="n">
-        <v>371.0094985961914</v>
-      </c>
-      <c r="I156" t="n">
-        <v>400.6961987304687</v>
-      </c>
-      <c r="J156" t="n">
-        <v>27.97414982387596</v>
-      </c>
     </row>
     <row r="157">
       <c r="A157" s="2" t="n">
@@ -5286,15 +4055,6 @@
       <c r="G157" t="n">
         <v>-0.02152157867491555</v>
       </c>
-      <c r="H157" t="n">
-        <v>367.2069992065429</v>
-      </c>
-      <c r="I157" t="n">
-        <v>399.5109985351563</v>
-      </c>
-      <c r="J157" t="n">
-        <v>30.74136317726003</v>
-      </c>
     </row>
     <row r="158">
       <c r="A158" s="2" t="n">
@@ -5318,15 +4078,6 @@
       <c r="G158" t="n">
         <v>-0.0838955952220366</v>
       </c>
-      <c r="H158" t="n">
-        <v>362.4894989013672</v>
-      </c>
-      <c r="I158" t="n">
-        <v>397.5471984863281</v>
-      </c>
-      <c r="J158" t="n">
-        <v>21.559900466005</v>
-      </c>
     </row>
     <row r="159">
       <c r="A159" s="2" t="n">
@@ -5350,15 +4101,6 @@
       <c r="G159" t="n">
         <v>-0.03963012048799908</v>
       </c>
-      <c r="H159" t="n">
-        <v>357.1249984741211</v>
-      </c>
-      <c r="I159" t="n">
-        <v>394.867798461914</v>
-      </c>
-      <c r="J159" t="n">
-        <v>21.84337908444151</v>
-      </c>
     </row>
     <row r="160">
       <c r="A160" s="2" t="n">
@@ -5382,15 +4124,6 @@
       <c r="G160" t="n">
         <v>-0.03043320480549028</v>
       </c>
-      <c r="H160" t="n">
-        <v>351.7674987792969</v>
-      </c>
-      <c r="I160" t="n">
-        <v>392.1447985839844</v>
-      </c>
-      <c r="J160" t="n">
-        <v>21.16141709776829</v>
-      </c>
     </row>
     <row r="161">
       <c r="A161" s="2" t="n">
@@ -5414,15 +4147,6 @@
       <c r="G161" t="n">
         <v>0.03912040539724382</v>
       </c>
-      <c r="H161" t="n">
-        <v>346.4024993896484</v>
-      </c>
-      <c r="I161" t="n">
-        <v>389.2797985839844</v>
-      </c>
-      <c r="J161" t="n">
-        <v>28.34427707833107</v>
-      </c>
     </row>
     <row r="162">
       <c r="A162" s="2" t="n">
@@ -5446,15 +4170,6 @@
       <c r="G162" t="n">
         <v>-0.02843203214376444</v>
       </c>
-      <c r="H162" t="n">
-        <v>340.4049987792969</v>
-      </c>
-      <c r="I162" t="n">
-        <v>385.7123986816407</v>
-      </c>
-      <c r="J162" t="n">
-        <v>28.80964646436969</v>
-      </c>
     </row>
     <row r="163">
       <c r="A163" s="2" t="n">
@@ -5478,15 +4193,6 @@
       <c r="G163" t="n">
         <v>-0.04429996705409467</v>
       </c>
-      <c r="H163" t="n">
-        <v>334.8229995727539</v>
-      </c>
-      <c r="I163" t="n">
-        <v>381.5559991455078</v>
-      </c>
-      <c r="J163" t="n">
-        <v>30.70403814467333</v>
-      </c>
     </row>
     <row r="164">
       <c r="A164" s="2" t="n">
@@ -5510,15 +4216,6 @@
       <c r="G164" t="n">
         <v>0.02595205608305928</v>
       </c>
-      <c r="H164" t="n">
-        <v>329.1675003051758</v>
-      </c>
-      <c r="I164" t="n">
-        <v>378.3353991699219</v>
-      </c>
-      <c r="J164" t="n">
-        <v>30.25111756059266</v>
-      </c>
     </row>
     <row r="165">
       <c r="A165" s="2" t="n">
@@ -5542,15 +4239,6 @@
       <c r="G165" t="n">
         <v>-0.05607306898689191</v>
       </c>
-      <c r="H165" t="n">
-        <v>323.4315002441406</v>
-      </c>
-      <c r="I165" t="n">
-        <v>374.8809991455078</v>
-      </c>
-      <c r="J165" t="n">
-        <v>17.334186109577</v>
-      </c>
     </row>
     <row r="166">
       <c r="A166" s="2" t="n">
@@ -5574,15 +4262,6 @@
       <c r="G166" t="n">
         <v>-0.002960708837181247</v>
       </c>
-      <c r="H166" t="n">
-        <v>317.8490005493164</v>
-      </c>
-      <c r="I166" t="n">
-        <v>371.7131994628906</v>
-      </c>
-      <c r="J166" t="n">
-        <v>17.25132410890818</v>
-      </c>
     </row>
     <row r="167">
       <c r="A167" s="2" t="n">
@@ -5606,15 +4285,6 @@
       <c r="G167" t="n">
         <v>-0.1542620682219512</v>
       </c>
-      <c r="H167" t="n">
-        <v>310.8755004882813</v>
-      </c>
-      <c r="I167" t="n">
-        <v>367.54419921875</v>
-      </c>
-      <c r="J167" t="n">
-        <v>13.55501954631907</v>
-      </c>
     </row>
     <row r="168">
       <c r="A168" s="2" t="n">
@@ -5638,15 +4308,6 @@
       <c r="G168" t="n">
         <v>0.03794736964295597</v>
       </c>
-      <c r="H168" t="n">
-        <v>304.8680000305176</v>
-      </c>
-      <c r="I168" t="n">
-        <v>362.9101992797852</v>
-      </c>
-      <c r="J168" t="n">
-        <v>14.4902216442858</v>
-      </c>
     </row>
     <row r="169">
       <c r="A169" s="2" t="n">
@@ -5670,15 +4331,6 @@
       <c r="G169" t="n">
         <v>0.0759389121683911</v>
       </c>
-      <c r="H169" t="n">
-        <v>300.8474998474121</v>
-      </c>
-      <c r="I169" t="n">
-        <v>358.7893991088867</v>
-      </c>
-      <c r="J169" t="n">
-        <v>22.65267267859464</v>
-      </c>
     </row>
     <row r="170">
       <c r="A170" s="2" t="n">
@@ -5702,15 +4354,6 @@
       <c r="G170" t="n">
         <v>-0.02986820819658198</v>
       </c>
-      <c r="H170" t="n">
-        <v>296.0559989929199</v>
-      </c>
-      <c r="I170" t="n">
-        <v>354.9697988891601</v>
-      </c>
-      <c r="J170" t="n">
-        <v>23.77686603346288</v>
-      </c>
     </row>
     <row r="171">
       <c r="A171" s="2" t="n">
@@ -5734,15 +4377,6 @@
       <c r="G171" t="n">
         <v>0.03864053238644471</v>
       </c>
-      <c r="H171" t="n">
-        <v>290.7579986572266</v>
-      </c>
-      <c r="I171" t="n">
-        <v>351.6211987304687</v>
-      </c>
-      <c r="J171" t="n">
-        <v>28.48672609288698</v>
-      </c>
     </row>
     <row r="172">
       <c r="A172" s="2" t="n">
@@ -5766,15 +4400,6 @@
       <c r="G172" t="n">
         <v>-0.04788383640805238</v>
       </c>
-      <c r="H172" t="n">
-        <v>284.8664985656739</v>
-      </c>
-      <c r="I172" t="n">
-        <v>348.3045986938477</v>
-      </c>
-      <c r="J172" t="n">
-        <v>31.10528012849956</v>
-      </c>
     </row>
     <row r="173">
       <c r="A173" s="2" t="n">
@@ -5798,15 +4423,6 @@
       <c r="G173" t="n">
         <v>-0.05335909096824687</v>
       </c>
-      <c r="H173" t="n">
-        <v>278.4264991760254</v>
-      </c>
-      <c r="I173" t="n">
-        <v>345.2251986694336</v>
-      </c>
-      <c r="J173" t="n">
-        <v>30.97879972224837</v>
-      </c>
     </row>
     <row r="174">
       <c r="A174" s="2" t="n">
@@ -5830,15 +4446,6 @@
       <c r="G174" t="n">
         <v>0.04682438935721978</v>
       </c>
-      <c r="H174" t="n">
-        <v>272.1914993286133</v>
-      </c>
-      <c r="I174" t="n">
-        <v>341.7335986328125</v>
-      </c>
-      <c r="J174" t="n">
-        <v>36.7443181095078</v>
-      </c>
     </row>
     <row r="175">
       <c r="A175" s="2" t="n">
@@ -5862,15 +4469,6 @@
       <c r="G175" t="n">
         <v>0.00169589542715709</v>
       </c>
-      <c r="H175" t="n">
-        <v>266.2844993591308</v>
-      </c>
-      <c r="I175" t="n">
-        <v>338.2377987670898</v>
-      </c>
-      <c r="J175" t="n">
-        <v>32.62467505429434</v>
-      </c>
     </row>
     <row r="176">
       <c r="A176" s="2" t="n">
@@ -5894,15 +4492,6 @@
       <c r="G176" t="n">
         <v>0.05269623506518384</v>
       </c>
-      <c r="H176" t="n">
-        <v>261.8300003051758</v>
-      </c>
-      <c r="I176" t="n">
-        <v>335.3247991943359</v>
-      </c>
-      <c r="J176" t="n">
-        <v>39.26138858253482</v>
-      </c>
     </row>
     <row r="177">
       <c r="A177" s="2" t="n">
@@ -5926,15 +4515,6 @@
       <c r="G177" t="n">
         <v>0.1193358012680052</v>
       </c>
-      <c r="H177" t="n">
-        <v>259.2230010986328</v>
-      </c>
-      <c r="I177" t="n">
-        <v>332.9937994384766</v>
-      </c>
-      <c r="J177" t="n">
-        <v>51.72170840154182</v>
-      </c>
     </row>
     <row r="178">
       <c r="A178" s="2" t="n">
@@ -5958,15 +4538,6 @@
       <c r="G178" t="n">
         <v>0.03502280788451673</v>
       </c>
-      <c r="H178" t="n">
-        <v>258.4900024414063</v>
-      </c>
-      <c r="I178" t="n">
-        <v>330.8617999267578</v>
-      </c>
-      <c r="J178" t="n">
-        <v>52.41582222755768</v>
-      </c>
     </row>
     <row r="179">
       <c r="A179" s="2" t="n">
@@ -5990,15 +4561,6 @@
       <c r="G179" t="n">
         <v>-0.05580626179068926</v>
       </c>
-      <c r="H179" t="n">
-        <v>257.5530029296875</v>
-      </c>
-      <c r="I179" t="n">
-        <v>328.2367999267578</v>
-      </c>
-      <c r="J179" t="n">
-        <v>52.29562806093099</v>
-      </c>
     </row>
     <row r="180">
       <c r="A180" s="2" t="n">
@@ -6022,15 +4584,6 @@
       <c r="G180" t="n">
         <v>0.003932982922225881</v>
       </c>
-      <c r="H180" t="n">
-        <v>257.1120025634766</v>
-      </c>
-      <c r="I180" t="n">
-        <v>325.7722003173828</v>
-      </c>
-      <c r="J180" t="n">
-        <v>52.78457769354657</v>
-      </c>
     </row>
     <row r="181">
       <c r="A181" s="2" t="n">
@@ -6054,15 +4607,6 @@
       <c r="G181" t="n">
         <v>-0.03507493471452938</v>
       </c>
-      <c r="H181" t="n">
-        <v>255.6405014038086</v>
-      </c>
-      <c r="I181" t="n">
-        <v>322.4788000488281</v>
-      </c>
-      <c r="J181" t="n">
-        <v>63.19479108267716</v>
-      </c>
     </row>
     <row r="182">
       <c r="A182" s="2" t="n">
@@ -6086,15 +4630,6 @@
       <c r="G182" t="n">
         <v>-0.01665712135910979</v>
       </c>
-      <c r="H182" t="n">
-        <v>254.3660018920899</v>
-      </c>
-      <c r="I182" t="n">
-        <v>319.3855999755859</v>
-      </c>
-      <c r="J182" t="n">
-        <v>59.34964471211322</v>
-      </c>
     </row>
     <row r="183">
       <c r="A183" s="2" t="n">
@@ -6118,15 +4653,6 @@
       <c r="G183" t="n">
         <v>0.03588511985473652</v>
       </c>
-      <c r="H183" t="n">
-        <v>254.1870010375977</v>
-      </c>
-      <c r="I183" t="n">
-        <v>316.2247998046875</v>
-      </c>
-      <c r="J183" t="n">
-        <v>57.04210403489001</v>
-      </c>
     </row>
     <row r="184">
       <c r="A184" s="2" t="n">
@@ -6150,15 +4676,6 @@
       <c r="G184" t="n">
         <v>0.05326685079977622</v>
       </c>
-      <c r="H184" t="n">
-        <v>254.3700012207031</v>
-      </c>
-      <c r="I184" t="n">
-        <v>313.3985998535156</v>
-      </c>
-      <c r="J184" t="n">
-        <v>63.88595670219329</v>
-      </c>
     </row>
     <row r="185">
       <c r="A185" s="2" t="n">
@@ -6182,15 +4699,6 @@
       <c r="G185" t="n">
         <v>-0.05474611137253549</v>
       </c>
-      <c r="H185" t="n">
-        <v>254.5615005493164</v>
-      </c>
-      <c r="I185" t="n">
-        <v>310.4420001220703</v>
-      </c>
-      <c r="J185" t="n">
-        <v>55.48509723870204</v>
-      </c>
     </row>
     <row r="186">
       <c r="A186" s="2" t="n">
@@ -6214,15 +4722,6 @@
       <c r="G186" t="n">
         <v>-0.1041978682681468</v>
       </c>
-      <c r="H186" t="n">
-        <v>253.3994995117187</v>
-      </c>
-      <c r="I186" t="n">
-        <v>306.9829998779297</v>
-      </c>
-      <c r="J186" t="n">
-        <v>50.40903262318778</v>
-      </c>
     </row>
     <row r="187">
       <c r="A187" s="2" t="n">
@@ -6246,15 +4745,6 @@
       <c r="G187" t="n">
         <v>-0.02564423663480953</v>
       </c>
-      <c r="H187" t="n">
-        <v>253.9564994812012</v>
-      </c>
-      <c r="I187" t="n">
-        <v>303.517200012207</v>
-      </c>
-      <c r="J187" t="n">
-        <v>52.38893324369187</v>
-      </c>
     </row>
     <row r="188">
       <c r="A188" s="2" t="n">
@@ -6278,15 +4768,6 @@
       <c r="G188" t="n">
         <v>-0.04899478333715857</v>
       </c>
-      <c r="H188" t="n">
-        <v>253.520499420166</v>
-      </c>
-      <c r="I188" t="n">
-        <v>300.0114001464844</v>
-      </c>
-      <c r="J188" t="n">
-        <v>45.83085306145372</v>
-      </c>
     </row>
     <row r="189">
       <c r="A189" s="2" t="n">
@@ -6310,15 +4791,6 @@
       <c r="G189" t="n">
         <v>0.2268998983962454</v>
       </c>
-      <c r="H189" t="n">
-        <v>254.7260002136231</v>
-      </c>
-      <c r="I189" t="n">
-        <v>297.4936004638672</v>
-      </c>
-      <c r="J189" t="n">
-        <v>58.24917501770583</v>
-      </c>
     </row>
     <row r="190">
       <c r="A190" s="2" t="n">
@@ -6342,15 +4814,6 @@
       <c r="G190" t="n">
         <v>-0.07274069589492627</v>
       </c>
-      <c r="H190" t="n">
-        <v>255.3120002746582</v>
-      </c>
-      <c r="I190" t="n">
-        <v>294.7596002197266</v>
-      </c>
-      <c r="J190" t="n">
-        <v>50.81930500742747</v>
-      </c>
     </row>
     <row r="191">
       <c r="A191" s="2" t="n">
@@ -6374,15 +4837,6 @@
       <c r="G191" t="n">
         <v>-0.0003565623615963132</v>
       </c>
-      <c r="H191" t="n">
-        <v>255.4285003662109</v>
-      </c>
-      <c r="I191" t="n">
-        <v>291.8002001953125</v>
-      </c>
-      <c r="J191" t="n">
-        <v>43.33333125306288</v>
-      </c>
     </row>
     <row r="192">
       <c r="A192" s="2" t="n">
@@ -6406,15 +4860,6 @@
       <c r="G192" t="n">
         <v>0.000158569003642306</v>
       </c>
-      <c r="H192" t="n">
-        <v>256.1455009460449</v>
-      </c>
-      <c r="I192" t="n">
-        <v>288.7552001953125</v>
-      </c>
-      <c r="J192" t="n">
-        <v>40.37334069252826</v>
-      </c>
     </row>
     <row r="193">
       <c r="A193" s="2" t="n">
@@ -6438,15 +4883,6 @@
       <c r="G193" t="n">
         <v>0.0069744183248166</v>
       </c>
-      <c r="H193" t="n">
-        <v>257.5855010986328</v>
-      </c>
-      <c r="I193" t="n">
-        <v>286.1638003540039</v>
-      </c>
-      <c r="J193" t="n">
-        <v>44.76890150004247</v>
-      </c>
     </row>
     <row r="194">
       <c r="A194" s="2" t="n">
@@ -6470,15 +4906,6 @@
       <c r="G194" t="n">
         <v>-0.04942740359854259</v>
       </c>
-      <c r="H194" t="n">
-        <v>257.8700012207031</v>
-      </c>
-      <c r="I194" t="n">
-        <v>283.1506005859375</v>
-      </c>
-      <c r="J194" t="n">
-        <v>41.3744143026149</v>
-      </c>
     </row>
     <row r="195">
       <c r="A195" s="2" t="n">
@@ -6502,15 +4929,6 @@
       <c r="G195" t="n">
         <v>-0.0007452201709629014</v>
       </c>
-      <c r="H195" t="n">
-        <v>258.1255012512207</v>
-      </c>
-      <c r="I195" t="n">
-        <v>280.4146002197265</v>
-      </c>
-      <c r="J195" t="n">
-        <v>43.61396167501861</v>
-      </c>
     </row>
     <row r="196">
       <c r="A196" s="2" t="n">
@@ -6534,15 +4952,6 @@
       <c r="G196" t="n">
         <v>-0.05746362595919796</v>
       </c>
-      <c r="H196" t="n">
-        <v>257.0650009155273</v>
-      </c>
-      <c r="I196" t="n">
-        <v>277.4782000732422</v>
-      </c>
-      <c r="J196" t="n">
-        <v>41.35634054436053</v>
-      </c>
     </row>
     <row r="197">
       <c r="A197" s="2" t="n">
@@ -6566,15 +4975,6 @@
       <c r="G197" t="n">
         <v>0.04602198338770602</v>
       </c>
-      <c r="H197" t="n">
-        <v>255.0440002441406</v>
-      </c>
-      <c r="I197" t="n">
-        <v>275.0052001953125</v>
-      </c>
-      <c r="J197" t="n">
-        <v>41.7286146868468</v>
-      </c>
     </row>
     <row r="198">
       <c r="A198" s="2" t="n">
@@ -6598,15 +4998,6 @@
       <c r="G198" t="n">
         <v>0.0536622440095611</v>
       </c>
-      <c r="H198" t="n">
-        <v>253.173999786377</v>
-      </c>
-      <c r="I198" t="n">
-        <v>273.0054000854492</v>
-      </c>
-      <c r="J198" t="n">
-        <v>41.24083694412561</v>
-      </c>
     </row>
     <row r="199">
       <c r="A199" s="2" t="n">
@@ -6630,15 +5021,6 @@
       <c r="G199" t="n">
         <v>0.0349764859229853</v>
       </c>
-      <c r="H199" t="n">
-        <v>252.5465003967285</v>
-      </c>
-      <c r="I199" t="n">
-        <v>271.6256002807617</v>
-      </c>
-      <c r="J199" t="n">
-        <v>47.79349481918855</v>
-      </c>
     </row>
     <row r="200">
       <c r="A200" s="2" t="n">
@@ -6662,15 +5044,6 @@
       <c r="G200" t="n">
         <v>0.09803091011549903</v>
       </c>
-      <c r="H200" t="n">
-        <v>253.1375007629395</v>
-      </c>
-      <c r="I200" t="n">
-        <v>270.5944003295899</v>
-      </c>
-      <c r="J200" t="n">
-        <v>63.10607237476127</v>
-      </c>
     </row>
     <row r="201">
       <c r="A201" s="2" t="n">
@@ -6694,15 +5067,6 @@
       <c r="G201" t="n">
         <v>0.003263704635694253</v>
       </c>
-      <c r="H201" t="n">
-        <v>254.2540016174316</v>
-      </c>
-      <c r="I201" t="n">
-        <v>269.1932003784179</v>
-      </c>
-      <c r="J201" t="n">
-        <v>65.60997418280343</v>
-      </c>
     </row>
     <row r="202">
       <c r="A202" s="2" t="n">
@@ -6726,15 +5090,6 @@
       <c r="G202" t="n">
         <v>0.02151250101945879</v>
       </c>
-      <c r="H202" t="n">
-        <v>255.897501373291</v>
-      </c>
-      <c r="I202" t="n">
-        <v>267.9170004272461</v>
-      </c>
-      <c r="J202" t="n">
-        <v>71.50211001793518</v>
-      </c>
     </row>
     <row r="203">
       <c r="A203" s="2" t="n">
@@ -6758,15 +5113,6 @@
       <c r="G203" t="n">
         <v>-0.03379788089732105</v>
       </c>
-      <c r="H203" t="n">
-        <v>256.5825019836426</v>
-      </c>
-      <c r="I203" t="n">
-        <v>266.4780007934571</v>
-      </c>
-      <c r="J203" t="n">
-        <v>54.05867582077851</v>
-      </c>
     </row>
     <row r="204">
       <c r="A204" s="2" t="n">
@@ -6790,15 +5136,6 @@
       <c r="G204" t="n">
         <v>-0.005812356915055328</v>
       </c>
-      <c r="H204" t="n">
-        <v>256.4705009460449</v>
-      </c>
-      <c r="I204" t="n">
-        <v>264.8772006225586</v>
-      </c>
-      <c r="J204" t="n">
-        <v>63.44939392515166</v>
-      </c>
     </row>
     <row r="205">
       <c r="A205" s="2" t="n">
@@ -6822,15 +5159,6 @@
       <c r="G205" t="n">
         <v>0.02384857658425266</v>
       </c>
-      <c r="H205" t="n">
-        <v>257.467000579834</v>
-      </c>
-      <c r="I205" t="n">
-        <v>263.5334005737305</v>
-      </c>
-      <c r="J205" t="n">
-        <v>65.70091294610739</v>
-      </c>
     </row>
     <row r="206">
       <c r="A206" s="2" t="n">
@@ -6854,15 +5182,6 @@
       <c r="G206" t="n">
         <v>-0.02419825875222081</v>
       </c>
-      <c r="H206" t="n">
-        <v>259.5085014343261</v>
-      </c>
-      <c r="I206" t="n">
-        <v>262.3826010131836</v>
-      </c>
-      <c r="J206" t="n">
-        <v>61.82126495051266</v>
-      </c>
     </row>
     <row r="207">
       <c r="A207" s="2" t="n">
@@ -6886,15 +5205,6 @@
       <c r="G207" t="n">
         <v>-0.01751945868486726</v>
       </c>
-      <c r="H207" t="n">
-        <v>261.6115020751953</v>
-      </c>
-      <c r="I207" t="n">
-        <v>261.279001159668</v>
-      </c>
-      <c r="J207" t="n">
-        <v>58.76237872441305</v>
-      </c>
     </row>
     <row r="208">
       <c r="A208" s="2" t="n">
@@ -6918,15 +5228,6 @@
       <c r="G208" t="n">
         <v>0.003159597232260225</v>
       </c>
-      <c r="H208" t="n">
-        <v>264.3295021057129</v>
-      </c>
-      <c r="I208" t="n">
-        <v>260.7474014282226</v>
-      </c>
-      <c r="J208" t="n">
-        <v>65.8296045603313</v>
-      </c>
     </row>
     <row r="209">
       <c r="A209" s="2" t="n">
@@ -6950,15 +5251,6 @@
       <c r="G209" t="n">
         <v>0.03113462481177853</v>
       </c>
-      <c r="H209" t="n">
-        <v>264.9605018615723</v>
-      </c>
-      <c r="I209" t="n">
-        <v>260.6278018188477</v>
-      </c>
-      <c r="J209" t="n">
-        <v>68.42195154140563</v>
-      </c>
     </row>
     <row r="210">
       <c r="A210" s="2" t="n">
@@ -6982,15 +5274,6 @@
       <c r="G210" t="n">
         <v>0.04718770485146129</v>
       </c>
-      <c r="H210" t="n">
-        <v>267.2535026550293</v>
-      </c>
-      <c r="I210" t="n">
-        <v>260.9540017700195</v>
-      </c>
-      <c r="J210" t="n">
-        <v>80.11064245345744</v>
-      </c>
     </row>
     <row r="211">
       <c r="A211" s="2" t="n">
@@ -7014,15 +5297,6 @@
       <c r="G211" t="n">
         <v>0.06745790403815088</v>
       </c>
-      <c r="H211" t="n">
-        <v>270.5570030212402</v>
-      </c>
-      <c r="I211" t="n">
-        <v>261.4620016479492</v>
-      </c>
-      <c r="J211" t="n">
-        <v>81.62013665827344</v>
-      </c>
     </row>
     <row r="212">
       <c r="A212" s="2" t="n">
@@ -7046,15 +5320,6 @@
       <c r="G212" t="n">
         <v>0.04928074062685361</v>
       </c>
-      <c r="H212" t="n">
-        <v>274.6430030822754</v>
-      </c>
-      <c r="I212" t="n">
-        <v>262.4504019165039</v>
-      </c>
-      <c r="J212" t="n">
-        <v>82.0327542532396</v>
-      </c>
     </row>
     <row r="213">
       <c r="A213" s="2" t="n">
@@ -7078,15 +5343,6 @@
       <c r="G213" t="n">
         <v>0.04073991993646375</v>
       </c>
-      <c r="H213" t="n">
-        <v>279.3215026855469</v>
-      </c>
-      <c r="I213" t="n">
-        <v>263.9632015991211</v>
-      </c>
-      <c r="J213" t="n">
-        <v>82.67734062021431</v>
-      </c>
     </row>
     <row r="214">
       <c r="A214" s="2" t="n">
@@ -7110,15 +5366,6 @@
       <c r="G214" t="n">
         <v>-0.01397832907829855</v>
       </c>
-      <c r="H214" t="n">
-        <v>284.3850028991699</v>
-      </c>
-      <c r="I214" t="n">
-        <v>265.2376016235352</v>
-      </c>
-      <c r="J214" t="n">
-        <v>75.30832561918703</v>
-      </c>
     </row>
     <row r="215">
       <c r="A215" s="2" t="n">
@@ -7142,15 +5389,6 @@
       <c r="G215" t="n">
         <v>0.0208856061756566</v>
       </c>
-      <c r="H215" t="n">
-        <v>289.815503692627</v>
-      </c>
-      <c r="I215" t="n">
-        <v>266.9682015991211</v>
-      </c>
-      <c r="J215" t="n">
-        <v>76.58428318983707</v>
-      </c>
     </row>
     <row r="216">
       <c r="A216" s="2" t="n">
@@ -7174,15 +5412,6 @@
       <c r="G216" t="n">
         <v>-0.02254418652711487</v>
       </c>
-      <c r="H216" t="n">
-        <v>295.5450035095215</v>
-      </c>
-      <c r="I216" t="n">
-        <v>268.5566012573242</v>
-      </c>
-      <c r="J216" t="n">
-        <v>70.46606809288325</v>
-      </c>
     </row>
     <row r="217">
       <c r="A217" s="2" t="n">
@@ -7206,15 +5435,6 @@
       <c r="G217" t="n">
         <v>0.005057180873010214</v>
       </c>
-      <c r="H217" t="n">
-        <v>300.8375038146972</v>
-      </c>
-      <c r="I217" t="n">
-        <v>270.9900015258789</v>
-      </c>
-      <c r="J217" t="n">
-        <v>77.00595728982744</v>
-      </c>
     </row>
     <row r="218">
       <c r="A218" s="2" t="n">
@@ -7238,15 +5458,6 @@
       <c r="G218" t="n">
         <v>-0.02675822235776915</v>
       </c>
-      <c r="H218" t="n">
-        <v>305.0315032958985</v>
-      </c>
-      <c r="I218" t="n">
-        <v>273.0708013916015</v>
-      </c>
-      <c r="J218" t="n">
-        <v>72.22313734840559</v>
-      </c>
     </row>
     <row r="219">
       <c r="A219" s="2" t="n">
@@ -7270,15 +5481,6 @@
       <c r="G219" t="n">
         <v>0.01918598267113714</v>
       </c>
-      <c r="H219" t="n">
-        <v>309.1080032348633</v>
-      </c>
-      <c r="I219" t="n">
-        <v>274.9298016357422</v>
-      </c>
-      <c r="J219" t="n">
-        <v>72.16138809359762</v>
-      </c>
     </row>
     <row r="220">
       <c r="A220" s="2" t="n">
@@ -7302,15 +5504,6 @@
       <c r="G220" t="n">
         <v>-0.004984788190348977</v>
       </c>
-      <c r="H220" t="n">
-        <v>311.8275024414062</v>
-      </c>
-      <c r="I220" t="n">
-        <v>276.9030017089844</v>
-      </c>
-      <c r="J220" t="n">
-        <v>75.4216716220507</v>
-      </c>
     </row>
     <row r="221">
       <c r="A221" s="2" t="n">
@@ -7334,15 +5527,6 @@
       <c r="G221" t="n">
         <v>0.06939947711644767</v>
       </c>
-      <c r="H221" t="n">
-        <v>315.6780029296875</v>
-      </c>
-      <c r="I221" t="n">
-        <v>279.1612020874023</v>
-      </c>
-      <c r="J221" t="n">
-        <v>82.4606835128877</v>
-      </c>
     </row>
     <row r="222">
       <c r="A222" s="2" t="n">
@@ -7366,15 +5550,6 @@
       <c r="G222" t="n">
         <v>-0.01650643586254685</v>
       </c>
-      <c r="H222" t="n">
-        <v>318.9215026855469</v>
-      </c>
-      <c r="I222" t="n">
-        <v>281.5390020751953</v>
-      </c>
-      <c r="J222" t="n">
-        <v>78.82250100954775</v>
-      </c>
     </row>
     <row r="223">
       <c r="A223" s="2" t="n">
@@ -7398,15 +5573,6 @@
       <c r="G223" t="n">
         <v>0.004286911755287504</v>
       </c>
-      <c r="H223" t="n">
-        <v>322.7350021362305</v>
-      </c>
-      <c r="I223" t="n">
-        <v>284.201401977539</v>
-      </c>
-      <c r="J223" t="n">
-        <v>77.69581737872778</v>
-      </c>
     </row>
     <row r="224">
       <c r="A224" s="2" t="n">
@@ -7430,15 +5596,6 @@
       <c r="G224" t="n">
         <v>-0.03339564619395741</v>
       </c>
-      <c r="H224" t="n">
-        <v>326.0320022583008</v>
-      </c>
-      <c r="I224" t="n">
-        <v>286.4134017944336</v>
-      </c>
-      <c r="J224" t="n">
-        <v>68.33813513135067</v>
-      </c>
     </row>
     <row r="225">
       <c r="A225" s="2" t="n">
@@ -7462,15 +5619,6 @@
       <c r="G225" t="n">
         <v>-0.01088145559849063</v>
       </c>
-      <c r="H225" t="n">
-        <v>328.8060028076172</v>
-      </c>
-      <c r="I225" t="n">
-        <v>288.542001953125</v>
-      </c>
-      <c r="J225" t="n">
-        <v>60.56312814670069</v>
-      </c>
     </row>
     <row r="226">
       <c r="A226" s="2" t="n">
@@ -7494,15 +5642,6 @@
       <c r="G226" t="n">
         <v>0.004610541775392996</v>
       </c>
-      <c r="H226" t="n">
-        <v>332.0065017700196</v>
-      </c>
-      <c r="I226" t="n">
-        <v>290.4532015991211</v>
-      </c>
-      <c r="J226" t="n">
-        <v>55.05149385220444</v>
-      </c>
     </row>
     <row r="227">
       <c r="A227" s="2" t="n">
@@ -7526,15 +5665,6 @@
       <c r="G227" t="n">
         <v>-0.03549540073392177</v>
       </c>
-      <c r="H227" t="n">
-        <v>334.8415008544922</v>
-      </c>
-      <c r="I227" t="n">
-        <v>291.5264010620117</v>
-      </c>
-      <c r="J227" t="n">
-        <v>42.15125331319467</v>
-      </c>
     </row>
     <row r="228">
       <c r="A228" s="2" t="n">
@@ -7558,15 +5688,6 @@
       <c r="G228" t="n">
         <v>-0.1425989378908212</v>
       </c>
-      <c r="H228" t="n">
-        <v>335.2655014038086</v>
-      </c>
-      <c r="I228" t="n">
-        <v>291.4576010131836</v>
-      </c>
-      <c r="J228" t="n">
-        <v>29.54386486514356</v>
-      </c>
     </row>
     <row r="229">
       <c r="A229" s="2" t="n">
@@ -7590,15 +5711,6 @@
       <c r="G229" t="n">
         <v>0.03667018613899597</v>
       </c>
-      <c r="H229" t="n">
-        <v>335.7815017700195</v>
-      </c>
-      <c r="I229" t="n">
-        <v>291.9192013549805</v>
-      </c>
-      <c r="J229" t="n">
-        <v>31.13390164793597</v>
-      </c>
     </row>
     <row r="230">
       <c r="A230" s="2" t="n">
@@ -7622,15 +5734,6 @@
       <c r="G230" t="n">
         <v>0.04553761352840424</v>
       </c>
-      <c r="H230" t="n">
-        <v>336.2975006103516</v>
-      </c>
-      <c r="I230" t="n">
-        <v>292.6282009887695</v>
-      </c>
-      <c r="J230" t="n">
-        <v>38.89588226109567</v>
-      </c>
     </row>
     <row r="231">
       <c r="A231" s="2" t="n">
@@ -7654,15 +5757,6 @@
       <c r="G231" t="n">
         <v>0.05674382827003055</v>
       </c>
-      <c r="H231" t="n">
-        <v>336.6830001831055</v>
-      </c>
-      <c r="I231" t="n">
-        <v>293.879001159668</v>
-      </c>
-      <c r="J231" t="n">
-        <v>44.68110351055573</v>
-      </c>
     </row>
     <row r="232">
       <c r="A232" s="2" t="n">
@@ -7686,15 +5780,6 @@
       <c r="G232" t="n">
         <v>0.00104264571654733</v>
       </c>
-      <c r="H232" t="n">
-        <v>336.3009994506836</v>
-      </c>
-      <c r="I232" t="n">
-        <v>295.2244009399414</v>
-      </c>
-      <c r="J232" t="n">
-        <v>47.40510659397059</v>
-      </c>
     </row>
     <row r="233">
       <c r="A233" s="2" t="n">
@@ -7718,15 +5803,6 @@
       <c r="G233" t="n">
         <v>-0.02242443246166159</v>
       </c>
-      <c r="H233" t="n">
-        <v>334.8724990844727</v>
-      </c>
-      <c r="I233" t="n">
-        <v>296.2374008178711</v>
-      </c>
-      <c r="J233" t="n">
-        <v>43.09116490011074</v>
-      </c>
     </row>
     <row r="234">
       <c r="A234" s="2" t="n">
@@ -7750,15 +5826,6 @@
       <c r="G234" t="n">
         <v>0.01942907615441958</v>
       </c>
-      <c r="H234" t="n">
-        <v>333.9969985961914</v>
-      </c>
-      <c r="I234" t="n">
-        <v>297.0884005737305</v>
-      </c>
-      <c r="J234" t="n">
-        <v>45.70185665282677</v>
-      </c>
     </row>
     <row r="235">
       <c r="A235" s="2" t="n">
@@ -7782,15 +5849,6 @@
       <c r="G235" t="n">
         <v>0.01174266807933155</v>
       </c>
-      <c r="H235" t="n">
-        <v>332.9544982910156</v>
-      </c>
-      <c r="I235" t="n">
-        <v>298.3254006958008</v>
-      </c>
-      <c r="J235" t="n">
-        <v>38.23528911304182</v>
-      </c>
     </row>
     <row r="236">
       <c r="A236" s="2" t="n">
@@ -7814,15 +5872,6 @@
       <c r="G236" t="n">
         <v>-0.03882963749794621</v>
       </c>
-      <c r="H236" t="n">
-        <v>331.6674987792969</v>
-      </c>
-      <c r="I236" t="n">
-        <v>299.8638009643554</v>
-      </c>
-      <c r="J236" t="n">
-        <v>36.50761995318484</v>
-      </c>
     </row>
     <row r="237">
       <c r="A237" s="2" t="n">
@@ -7846,15 +5895,6 @@
       <c r="G237" t="n">
         <v>0.0180179597897272</v>
       </c>
-      <c r="H237" t="n">
-        <v>330.5789978027344</v>
-      </c>
-      <c r="I237" t="n">
-        <v>301.6390008544922</v>
-      </c>
-      <c r="J237" t="n">
-        <v>38.22195717262159</v>
-      </c>
     </row>
     <row r="238">
       <c r="A238" s="2" t="n">
@@ -7878,15 +5918,6 @@
       <c r="G238" t="n">
         <v>0.0003416111576173275</v>
       </c>
-      <c r="H238" t="n">
-        <v>329.9559982299805</v>
-      </c>
-      <c r="I238" t="n">
-        <v>303.6450009155274</v>
-      </c>
-      <c r="J238" t="n">
-        <v>41.47846988266417</v>
-      </c>
     </row>
     <row r="239">
       <c r="A239" s="2" t="n">
@@ -7910,15 +5941,6 @@
       <c r="G239" t="n">
         <v>0.08231930938729071</v>
       </c>
-      <c r="H239" t="n">
-        <v>330.3379974365234</v>
-      </c>
-      <c r="I239" t="n">
-        <v>305.1746005249024</v>
-      </c>
-      <c r="J239" t="n">
-        <v>51.81152598637165</v>
-      </c>
     </row>
     <row r="240">
       <c r="A240" s="2" t="n">
@@ -7942,15 +5964,6 @@
       <c r="G240" t="n">
         <v>-0.02354592069385564</v>
       </c>
-      <c r="H240" t="n">
-        <v>330.3944976806641</v>
-      </c>
-      <c r="I240" t="n">
-        <v>306.9360006713867</v>
-      </c>
-      <c r="J240" t="n">
-        <v>48.89509518022341</v>
-      </c>
     </row>
     <row r="241">
       <c r="A241" s="2" t="n">
@@ -7974,15 +5987,6 @@
       <c r="G241" t="n">
         <v>-0.037947582404945</v>
       </c>
-      <c r="H241" t="n">
-        <v>328.6274963378906</v>
-      </c>
-      <c r="I241" t="n">
-        <v>308.4408004760742</v>
-      </c>
-      <c r="J241" t="n">
-        <v>48.69686067996979</v>
-      </c>
     </row>
     <row r="242">
       <c r="A242" s="2" t="n">
@@ -8006,15 +6010,6 @@
       <c r="G242" t="n">
         <v>-0.005403721812350049</v>
       </c>
-      <c r="H242" t="n">
-        <v>327.0714965820313</v>
-      </c>
-      <c r="I242" t="n">
-        <v>309.9094003295899</v>
-      </c>
-      <c r="J242" t="n">
-        <v>66.16304332425506</v>
-      </c>
     </row>
     <row r="243">
       <c r="A243" s="2" t="n">
@@ -8038,15 +6033,6 @@
       <c r="G243" t="n">
         <v>-0.006599526995335614</v>
       </c>
-      <c r="H243" t="n">
-        <v>325.3314971923828</v>
-      </c>
-      <c r="I243" t="n">
-        <v>311.299800415039</v>
-      </c>
-      <c r="J243" t="n">
-        <v>61.99174825498201</v>
-      </c>
     </row>
     <row r="244">
       <c r="A244" s="2" t="n">
@@ -8070,15 +6056,6 @@
       <c r="G244" t="n">
         <v>-0.01844699542882278</v>
       </c>
-      <c r="H244" t="n">
-        <v>323.8914978027344</v>
-      </c>
-      <c r="I244" t="n">
-        <v>312.8220004272461</v>
-      </c>
-      <c r="J244" t="n">
-        <v>54.07834014212659</v>
-      </c>
     </row>
     <row r="245">
       <c r="A245" s="2" t="n">
@@ -8102,15 +6079,6 @@
       <c r="G245" t="n">
         <v>-0.05335897504131726</v>
       </c>
-      <c r="H245" t="n">
-        <v>321.792497253418</v>
-      </c>
-      <c r="I245" t="n">
-        <v>314.0088003540039</v>
-      </c>
-      <c r="J245" t="n">
-        <v>38.54279403887823</v>
-      </c>
     </row>
     <row r="246">
       <c r="A246" s="2" t="n">
@@ -8134,15 +6102,6 @@
       <c r="G246" t="n">
         <v>0.04968242780731846</v>
       </c>
-      <c r="H246" t="n">
-        <v>320.3614974975586</v>
-      </c>
-      <c r="I246" t="n">
-        <v>315.7718002319336</v>
-      </c>
-      <c r="J246" t="n">
-        <v>45.7003839284171</v>
-      </c>
     </row>
     <row r="247">
       <c r="A247" s="2" t="n">
@@ -8166,15 +6125,6 @@
       <c r="G247" t="n">
         <v>-0.0009503811144286889</v>
       </c>
-      <c r="H247" t="n">
-        <v>319.526498413086</v>
-      </c>
-      <c r="I247" t="n">
-        <v>317.3194003295898</v>
-      </c>
-      <c r="J247" t="n">
-        <v>48.41136582541748</v>
-      </c>
     </row>
     <row r="248">
       <c r="A248" s="2" t="n">
@@ -8198,15 +6148,6 @@
       <c r="G248" t="n">
         <v>-0.06789282780315342</v>
       </c>
-      <c r="H248" t="n">
-        <v>319.9884979248047</v>
-      </c>
-      <c r="I248" t="n">
-        <v>318.1834002685547</v>
-      </c>
-      <c r="J248" t="n">
-        <v>38.25533583506659</v>
-      </c>
     </row>
     <row r="249">
       <c r="A249" s="2" t="n">
@@ -8230,15 +6171,6 @@
       <c r="G249" t="n">
         <v>0.01316593551420042</v>
       </c>
-      <c r="H249" t="n">
-        <v>320.1219970703125</v>
-      </c>
-      <c r="I249" t="n">
-        <v>318.949400024414</v>
-      </c>
-      <c r="J249" t="n">
-        <v>38.27843823067456</v>
-      </c>
     </row>
     <row r="250">
       <c r="A250" s="2" t="n">
@@ -8262,15 +6194,6 @@
       <c r="G250" t="n">
         <v>-0.006480617479611372</v>
       </c>
-      <c r="H250" t="n">
-        <v>319.4869979858398</v>
-      </c>
-      <c r="I250" t="n">
-        <v>319.1679998779297</v>
-      </c>
-      <c r="J250" t="n">
-        <v>41.66191189007404</v>
-      </c>
     </row>
     <row r="251">
       <c r="A251" s="2" t="n">
@@ -8294,15 +6217,6 @@
       <c r="G251" t="n">
         <v>0.0472826483827995</v>
       </c>
-      <c r="H251" t="n">
-        <v>318.6759979248047</v>
-      </c>
-      <c r="I251" t="n">
-        <v>319.6477996826172</v>
-      </c>
-      <c r="J251" t="n">
-        <v>45.35256611793704</v>
-      </c>
     </row>
     <row r="252">
       <c r="A252" s="2" t="n">
@@ -8326,22 +6240,13 @@
       <c r="G252" t="n">
         <v>0.01174690904506881</v>
       </c>
-      <c r="H252" t="n">
-        <v>318.0299987792969</v>
-      </c>
-      <c r="I252" t="n">
-        <v>320.0773999023438</v>
-      </c>
-      <c r="J252" t="n">
-        <v>46.78606101384959</v>
-      </c>
     </row>
     <row r="253">
       <c r="A253" s="2" t="n">
         <v>45852</v>
       </c>
       <c r="B253" t="n">
-        <v>316.2901000976562</v>
+        <v>316.0499877929688</v>
       </c>
       <c r="C253" t="n">
         <v>322.5986022949219</v>
@@ -8353,19 +6258,10 @@
         <v>317.7300109863281</v>
       </c>
       <c r="F253" t="n">
-        <v>63108777</v>
+        <v>67146846</v>
       </c>
       <c r="G253" t="n">
-        <v>0.008867628609720013</v>
-      </c>
-      <c r="H253" t="n">
-        <v>317.8890045166016</v>
-      </c>
-      <c r="I253" t="n">
-        <v>320.7600018310547</v>
-      </c>
-      <c r="J253" t="n">
-        <v>35.3875892149088</v>
+        <v>0.008101744595786942</v>
       </c>
     </row>
   </sheetData>

</xml_diff>